<commit_message>
Links + API Ergänzungen
</commit_message>
<xml_diff>
--- a/BTR Tools Evaluation.xlsx
+++ b/BTR Tools Evaluation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="110">
   <si>
     <t>Fehlermanagement</t>
   </si>
@@ -317,14 +317,6 @@
   </si>
   <si>
     <t>INTERNE ADRESSE AUF CETEQ SERVER</t>
-  </si>
-  <si>
-    <t>• Insgesamt wirkt JIRA sehr ausgereift, leicht pflegbar / erweiterbar (Plugins) und hat eine gute Performance auf unserem Server.
-• Die Oberfläche ist strukturiert, Einsteiger werden möglicherweise von der Vielzahl an Funktionen "erschlagen".
-• Insbesondere die Traceability/Verlinkung (bzw. dessen Darstellung) zwischen Anforderungen, Test(-fällen) [mit RMsis] und Bugtracking lässt sich sehr gut einpflegen und nachverfolgen.
-• Gute Kompatibilität zu anderen Bugtracking Systemen (Migration) und Versionsverwaltungen (&gt; Konfigurationsmanagement?).
-• Sowohl JIRA als auch RMsis befinden sich weiterhin in Weiterentwicklung.
-• Inklsuive RMsis vergleichsweise teuer.</t>
   </si>
   <si>
     <t>27.01.2015 (2.2.8)</t>
@@ -376,6 +368,42 @@
   </si>
   <si>
     <t>Trac 1.0</t>
+  </si>
+  <si>
+    <t>• SpiraTest stellt eine verhältnismäßig (im Vgl. zu HPQC) günstige Allround-Lösung für Issue-Tracking, Test Case Management und Requirements Management dar.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Insgesamt wirkt JIRA sehr ausgereift, leicht pflegbar / erweiterbar (Plugins) und hat eine gute Performance auf unserem Server.
+• Die Oberfläche ist strukturiert, Einsteiger werden möglicherweise von der Vielzahl an Funktionen "erschlagen".
+• Insbesondere die Traceability/Verlinkung (bzw. dessen Darstellung) zwischen Anforderungen, Test(-fällen) [mit RMsis] und Bugtracking lässt sich sehr gut einpflegen und nachverfolgen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Traceabilitymatrix!)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+• Gute Kompatibilität zu anderen Bugtracking Systemen (Migration) und Versionsverwaltungen (&gt; Konfigurationsmanagement?).
+• Sowohl JIRA als auch RMsis befinden sich weiterhin in Weiterentwicklung.
+• Inklsuive RMsis vergleichsweise teuer.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -853,7 +881,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -868,6 +896,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -921,9 +952,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1295,6 +1323,9 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1311,6 +1342,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1610,35 +1647,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="topRight" activeCell="F10" sqref="F10:G10"/>
+      <selection pane="topRight" activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="29" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="5"/>
-    <col min="6" max="6" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="5" customWidth="1"/>
-    <col min="9" max="10" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="5" customWidth="1"/>
-    <col min="12" max="13" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" style="5"/>
-    <col min="16" max="16" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="7" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" style="7"/>
-    <col min="21" max="21" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="11.42578125" style="7"/>
-    <col min="24" max="24" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.42578125" style="7"/>
+    <col min="16" max="16" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="8" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="8"/>
+    <col min="21" max="21" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.42578125" style="8"/>
+    <col min="24" max="24" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1658,24 +1695,24 @@
       <c r="F1" s="124" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="96"/>
       <c r="I1" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="24" t="s">
         <v>65</v>
       </c>
       <c r="K1" s="96"/>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="20" t="s">
         <v>67</v>
       </c>
       <c r="M1" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="24" t="s">
         <v>67</v>
       </c>
       <c r="O1" s="96"/>
@@ -1692,14 +1729,14 @@
       <c r="T1" s="124" t="s">
         <v>72</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="21" t="s">
         <v>79</v>
       </c>
       <c r="V1" s="96"/>
       <c r="W1" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="X1" s="21" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1714,16 +1751,16 @@
       </c>
       <c r="E2" s="105"/>
       <c r="F2" s="142"/>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>74</v>
       </c>
       <c r="H2" s="97"/>
       <c r="I2" s="83"/>
-      <c r="J2" s="24"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="97"/>
-      <c r="L2" s="21"/>
+      <c r="L2" s="22"/>
       <c r="M2" s="83"/>
-      <c r="N2" s="24"/>
+      <c r="N2" s="25"/>
       <c r="O2" s="97"/>
       <c r="P2" s="142"/>
       <c r="Q2" s="84" t="s">
@@ -1734,12 +1771,12 @@
       </c>
       <c r="S2" s="97"/>
       <c r="T2" s="142"/>
-      <c r="U2" s="22" t="s">
+      <c r="U2" s="23" t="s">
         <v>76</v>
       </c>
       <c r="V2" s="97"/>
       <c r="W2" s="142"/>
-      <c r="X2" s="22" t="s">
+      <c r="X2" s="23" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1754,7 +1791,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="148" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" s="97"/>
       <c r="F3" s="143" t="s">
@@ -1827,17 +1864,17 @@
       <c r="I4" s="175" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="27" t="s">
         <v>66</v>
       </c>
       <c r="K4" s="99"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="26" t="s">
         <v>20</v>
       </c>
       <c r="M4" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="N4" s="27" t="s">
         <v>22</v>
       </c>
       <c r="O4" s="99"/>
@@ -1854,15 +1891,15 @@
       <c r="T4" s="144" t="s">
         <v>78</v>
       </c>
-      <c r="U4" s="26"/>
+      <c r="U4" s="27"/>
       <c r="V4" s="99"/>
       <c r="W4" s="133" t="s">
         <v>82</v>
       </c>
-      <c r="X4" s="26"/>
+      <c r="X4" s="27"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="165">
@@ -1876,7 +1913,7 @@
       </c>
       <c r="E5" s="97"/>
       <c r="F5" s="125" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="67">
         <v>41882</v>
@@ -1889,7 +1926,7 @@
         <v>41915</v>
       </c>
       <c r="K5" s="97"/>
-      <c r="L5" s="27"/>
+      <c r="L5" s="28"/>
       <c r="M5" s="165"/>
       <c r="N5" s="67"/>
       <c r="O5" s="97"/>
@@ -1914,7 +1951,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>93</v>
       </c>
       <c r="B6" s="184" t="str">
@@ -1939,12 +1976,27 @@
         <v>Link</v>
       </c>
       <c r="H6" s="97"/>
-      <c r="I6" s="165"/>
-      <c r="J6" s="67"/>
+      <c r="I6" s="184" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraTest/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="J6" s="184" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraTest/","Link")</f>
+        <v>Link</v>
+      </c>
       <c r="K6" s="97"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="165"/>
-      <c r="N6" s="67"/>
+      <c r="L6" s="193" t="str">
+        <f>HYPERLINK("http://www.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="M6" s="193" t="str">
+        <f>HYPERLINK("http://www.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="N6" s="193" t="str">
+        <f>HYPERLINK("http://www.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
       <c r="O6" s="97"/>
       <c r="P6" s="125"/>
       <c r="Q6" s="2"/>
@@ -1960,7 +2012,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="184"/>
@@ -1985,7 +2037,7 @@
       <c r="I7" s="165"/>
       <c r="J7" s="67"/>
       <c r="K7" s="97"/>
-      <c r="L7" s="27"/>
+      <c r="L7" s="28"/>
       <c r="M7" s="165"/>
       <c r="N7" s="67"/>
       <c r="O7" s="97"/>
@@ -2000,8 +2052,8 @@
       <c r="X7" s="87"/>
     </row>
     <row r="8" spans="1:24" ht="15">
-      <c r="A8" s="8" t="s">
-        <v>104</v>
+      <c r="A8" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="B8" s="184" t="str">
         <f>HYPERLINK("https://confluence.atlassian.com/display/JIRA/JIRA+Documentation","Link")</f>
@@ -2025,12 +2077,27 @@
         <v>Link</v>
       </c>
       <c r="H8" s="97"/>
-      <c r="I8" s="165"/>
-      <c r="J8" s="67"/>
+      <c r="I8" s="184" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraTest/Documentation.aspx","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="J8" s="184" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraTest/Documentation.aspx","Link")</f>
+        <v>Link</v>
+      </c>
       <c r="K8" s="97"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="165"/>
-      <c r="N8" s="67"/>
+      <c r="L8" s="193" t="str">
+        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="M8" s="193" t="str">
+        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="N8" s="193" t="str">
+        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
       <c r="O8" s="97"/>
       <c r="P8" s="125"/>
       <c r="Q8" s="2"/>
@@ -2043,8 +2110,8 @@
       <c r="X8" s="87"/>
     </row>
     <row r="9" spans="1:24" ht="15">
-      <c r="A9" s="8" t="s">
-        <v>105</v>
+      <c r="A9" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="B9" s="184" t="str">
         <f>HYPERLINK("https://confluence.atlassian.com/display/JIRA/JIRA+User%27s+Guide","Link")</f>
@@ -2068,12 +2135,27 @@
         <v>Link</v>
       </c>
       <c r="H9" s="97"/>
-      <c r="I9" s="165"/>
-      <c r="J9" s="67"/>
+      <c r="I9" s="184" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraDemo/Help/Frameset.aspx?section=1.%20Introduction","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="J9" s="184" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraDemo/Help/Frameset.aspx?section=1.%20Introduction","Link")</f>
+        <v>Link</v>
+      </c>
       <c r="K9" s="97"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="165"/>
-      <c r="N9" s="67"/>
+      <c r="L9" s="193" t="str">
+        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="M9" s="193" t="str">
+        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="N9" s="193" t="str">
+        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
       <c r="O9" s="97"/>
       <c r="P9" s="125"/>
       <c r="Q9" s="2"/>
@@ -2085,30 +2167,32 @@
       <c r="W9" s="145"/>
       <c r="X9" s="87"/>
     </row>
-    <row r="10" spans="1:24" s="11" customFormat="1" ht="313.5" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:24" s="12" customFormat="1" ht="313.5" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>97</v>
       </c>
       <c r="B10" s="189" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C10" s="190"/>
       <c r="D10" s="191"/>
       <c r="E10" s="98"/>
       <c r="F10" s="189" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G10" s="191"/>
       <c r="H10" s="98"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="29"/>
+      <c r="I10" s="189" t="s">
+        <v>108</v>
+      </c>
+      <c r="J10" s="191"/>
       <c r="K10" s="98"/>
-      <c r="L10" s="28"/>
+      <c r="L10" s="193"/>
       <c r="M10" s="166"/>
       <c r="N10" s="29"/>
       <c r="O10" s="98"/>
       <c r="P10" s="126"/>
-      <c r="Q10" s="10"/>
+      <c r="Q10" s="11"/>
       <c r="R10" s="91"/>
       <c r="S10" s="98"/>
       <c r="T10" s="126"/>
@@ -2149,12 +2233,12 @@
       <c r="X11" s="50"/>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="167"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="151"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="152"/>
       <c r="E12" s="97"/>
       <c r="F12" s="135"/>
       <c r="G12" s="36"/>
@@ -2167,7 +2251,7 @@
       <c r="N12" s="34"/>
       <c r="O12" s="97"/>
       <c r="P12" s="135"/>
-      <c r="Q12" s="14"/>
+      <c r="Q12" s="15"/>
       <c r="R12" s="59"/>
       <c r="S12" s="97"/>
       <c r="T12" s="136"/>
@@ -2177,7 +2261,7 @@
       <c r="X12" s="36"/>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="167"/>
@@ -2195,7 +2279,7 @@
       <c r="N13" s="34"/>
       <c r="O13" s="97"/>
       <c r="P13" s="129"/>
-      <c r="Q13" s="13"/>
+      <c r="Q13" s="14"/>
       <c r="R13" s="60"/>
       <c r="S13" s="97"/>
       <c r="T13" s="129"/>
@@ -2205,7 +2289,7 @@
       <c r="X13" s="33"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="58"/>
@@ -2223,7 +2307,7 @@
       <c r="N14" s="34"/>
       <c r="O14" s="97"/>
       <c r="P14" s="136"/>
-      <c r="Q14" s="12"/>
+      <c r="Q14" s="13"/>
       <c r="R14" s="167"/>
       <c r="S14" s="97"/>
       <c r="T14" s="136"/>
@@ -2260,43 +2344,43 @@
       <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="194" t="s">
+      <c r="B16" s="195" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="195"/>
-      <c r="D16" s="196"/>
+      <c r="C16" s="196"/>
+      <c r="D16" s="197"/>
       <c r="E16" s="97"/>
-      <c r="F16" s="194" t="s">
+      <c r="F16" s="195" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="196"/>
+      <c r="G16" s="197"/>
       <c r="H16" s="97"/>
-      <c r="I16" s="194" t="s">
+      <c r="I16" s="195" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="196"/>
+      <c r="J16" s="197"/>
       <c r="K16" s="97"/>
-      <c r="L16" s="194" t="s">
+      <c r="L16" s="195" t="s">
         <v>69</v>
       </c>
-      <c r="M16" s="195"/>
-      <c r="N16" s="196"/>
+      <c r="M16" s="196"/>
+      <c r="N16" s="197"/>
       <c r="O16" s="97"/>
-      <c r="P16" s="194" t="s">
+      <c r="P16" s="195" t="s">
         <v>70</v>
       </c>
-      <c r="Q16" s="195"/>
-      <c r="R16" s="196"/>
+      <c r="Q16" s="196"/>
+      <c r="R16" s="197"/>
       <c r="S16" s="97"/>
-      <c r="T16" s="194" t="s">
+      <c r="T16" s="195" t="s">
         <v>81</v>
       </c>
-      <c r="U16" s="196"/>
+      <c r="U16" s="197"/>
       <c r="V16" s="97"/>
-      <c r="W16" s="194" t="s">
+      <c r="W16" s="195" t="s">
         <v>70</v>
       </c>
-      <c r="X16" s="196"/>
+      <c r="X16" s="197"/>
     </row>
     <row r="17" spans="1:24">
       <c r="B17" s="90"/>
@@ -2323,7 +2407,7 @@
       <c r="X17" s="31"/>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="59"/>
@@ -2341,7 +2425,7 @@
       <c r="N18" s="36"/>
       <c r="O18" s="97"/>
       <c r="P18" s="129"/>
-      <c r="Q18" s="14"/>
+      <c r="Q18" s="15"/>
       <c r="R18" s="59"/>
       <c r="S18" s="97"/>
       <c r="T18" s="129"/>
@@ -2375,7 +2459,7 @@
       <c r="X19" s="38"/>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="167"/>
@@ -2426,7 +2510,7 @@
       <c r="X21" s="31"/>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="168" t="s">
@@ -2466,7 +2550,7 @@
       <c r="P22" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="Q22" s="6" t="s">
+      <c r="Q22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="R22" s="178" t="s">
@@ -2488,8 +2572,8 @@
       </c>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="7" t="s">
-        <v>106</v>
+      <c r="A23" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="B23" s="168"/>
       <c r="C23" s="115"/>
@@ -2506,7 +2590,7 @@
       <c r="N23" s="36"/>
       <c r="O23" s="99"/>
       <c r="P23" s="129"/>
-      <c r="Q23" s="12"/>
+      <c r="Q23" s="13"/>
       <c r="R23" s="167"/>
       <c r="S23" s="99"/>
       <c r="T23" s="129"/>
@@ -2540,7 +2624,7 @@
       <c r="X24" s="31"/>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="93" t="s">
@@ -2556,24 +2640,24 @@
       <c r="F25" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="27" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="97"/>
       <c r="I25" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="27" t="s">
         <v>10</v>
       </c>
       <c r="K25" s="97"/>
-      <c r="L25" s="25" t="s">
+      <c r="L25" s="26" t="s">
         <v>11</v>
       </c>
       <c r="M25" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="N25" s="26" t="s">
+      <c r="N25" s="27" t="s">
         <v>11</v>
       </c>
       <c r="O25" s="97"/>
@@ -2602,7 +2686,7 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="93" t="s">
@@ -2616,24 +2700,24 @@
       <c r="F26" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="27" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="97"/>
       <c r="I26" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="27" t="s">
         <v>10</v>
       </c>
       <c r="K26" s="97"/>
-      <c r="L26" s="25" t="s">
+      <c r="L26" s="26" t="s">
         <v>11</v>
       </c>
       <c r="M26" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="N26" s="26" t="s">
+      <c r="N26" s="27" t="s">
         <v>11</v>
       </c>
       <c r="O26" s="97"/>
@@ -2667,10 +2751,10 @@
       <c r="D27" s="149"/>
       <c r="E27" s="97"/>
       <c r="F27" s="133"/>
-      <c r="G27" s="26"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="97"/>
       <c r="I27" s="93"/>
-      <c r="J27" s="26"/>
+      <c r="J27" s="27"/>
       <c r="K27" s="97"/>
       <c r="L27" s="30"/>
       <c r="M27" s="90"/>
@@ -2712,42 +2796,63 @@
       <c r="W28" s="134"/>
       <c r="X28" s="53"/>
     </row>
-    <row r="29" spans="1:24" ht="15">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:24" s="1" customFormat="1" ht="15">
+      <c r="A29" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="197" t="str">
+      <c r="B29" s="198" t="str">
         <f>HYPERLINK("https://docs.atlassian.com/jira/REST/latest/","REST")</f>
         <v>REST</v>
       </c>
-      <c r="C29" s="198" t="str">
+      <c r="C29" s="199" t="str">
         <f>HYPERLINK("https://docs.atlassian.com/jira/REST/latest/","REST")</f>
         <v>REST</v>
       </c>
-      <c r="D29" s="154"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="129"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="167"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="97"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="97"/>
-      <c r="P29" s="129"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="167"/>
-      <c r="S29" s="97"/>
-      <c r="T29" s="129"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="97"/>
-      <c r="W29" s="129"/>
-      <c r="X29" s="34"/>
+      <c r="D29" s="156"/>
+      <c r="E29" s="99"/>
+      <c r="F29" s="200" t="str">
+        <f>HYPERLINK("https://wiki.mozilla.org/Bugzilla:REST_API","REST")</f>
+        <v>REST</v>
+      </c>
+      <c r="G29" s="201" t="str">
+        <f>HYPERLINK("https://wiki.mozilla.org/Testopia:Documentation","XMLRPC")</f>
+        <v>XMLRPC</v>
+      </c>
+      <c r="H29" s="99"/>
+      <c r="I29" s="198" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraDemo/Services/v4_0/RestService.aspx","REST")</f>
+        <v>REST</v>
+      </c>
+      <c r="J29" s="198" t="str">
+        <f>HYPERLINK("http://www.inflectra.com/SpiraDemo/Services/v4_0/RestService.aspx","REST")</f>
+        <v>REST</v>
+      </c>
+      <c r="K29" s="99"/>
+      <c r="L29" s="201" t="str">
+        <f>HYPERLINK("http://support.practitest.com/customer/portal/topics/394423-api/articles","REST")</f>
+        <v>REST</v>
+      </c>
+      <c r="M29" s="201" t="str">
+        <f>HYPERLINK("http://support.practitest.com/customer/portal/topics/394423-api/articles","REST")</f>
+        <v>REST</v>
+      </c>
+      <c r="N29" s="201" t="str">
+        <f>HYPERLINK("http://support.practitest.com/customer/portal/topics/394423-api/articles","REST")</f>
+        <v>REST</v>
+      </c>
+      <c r="O29" s="99"/>
+      <c r="P29" s="132"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="168"/>
+      <c r="S29" s="99"/>
+      <c r="T29" s="132"/>
+      <c r="U29" s="68"/>
+      <c r="V29" s="99"/>
+      <c r="W29" s="132"/>
+      <c r="X29" s="68"/>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="90"/>
       <c r="C30" s="114"/>
       <c r="D30" s="153"/>
@@ -2772,7 +2877,7 @@
       <c r="X30" s="31"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B31" s="90"/>
@@ -2799,7 +2904,7 @@
       <c r="X31" s="31"/>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="167"/>
@@ -2817,7 +2922,7 @@
       <c r="N32" s="34"/>
       <c r="O32" s="97"/>
       <c r="P32" s="135"/>
-      <c r="Q32" s="12"/>
+      <c r="Q32" s="13"/>
       <c r="R32" s="167"/>
       <c r="S32" s="97"/>
       <c r="T32" s="129"/>
@@ -2845,7 +2950,7 @@
       <c r="N33" s="36"/>
       <c r="O33" s="97"/>
       <c r="P33" s="135"/>
-      <c r="Q33" s="14"/>
+      <c r="Q33" s="15"/>
       <c r="R33" s="59"/>
       <c r="S33" s="97"/>
       <c r="T33" s="135"/>
@@ -2875,7 +2980,7 @@
       <c r="N34" s="34"/>
       <c r="O34" s="97"/>
       <c r="P34" s="135"/>
-      <c r="Q34" s="12"/>
+      <c r="Q34" s="13"/>
       <c r="R34" s="167"/>
       <c r="S34" s="97"/>
       <c r="T34" s="129"/>
@@ -2885,7 +2990,7 @@
       <c r="X34" s="88"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="167"/>
@@ -2903,7 +3008,7 @@
       <c r="N35" s="36"/>
       <c r="O35" s="97"/>
       <c r="P35" s="135"/>
-      <c r="Q35" s="12"/>
+      <c r="Q35" s="13"/>
       <c r="R35" s="167"/>
       <c r="S35" s="97"/>
       <c r="T35" s="129"/>
@@ -2913,7 +3018,7 @@
       <c r="X35" s="88"/>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B36" s="167"/>
@@ -2931,7 +3036,7 @@
       <c r="N36" s="34"/>
       <c r="O36" s="97"/>
       <c r="P36" s="135"/>
-      <c r="Q36" s="12"/>
+      <c r="Q36" s="13"/>
       <c r="R36" s="167"/>
       <c r="S36" s="97"/>
       <c r="T36" s="129"/>
@@ -2941,7 +3046,7 @@
       <c r="X36" s="88"/>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="167"/>
@@ -2959,7 +3064,7 @@
       <c r="N37" s="36"/>
       <c r="O37" s="97"/>
       <c r="P37" s="135"/>
-      <c r="Q37" s="12"/>
+      <c r="Q37" s="13"/>
       <c r="R37" s="167"/>
       <c r="S37" s="97"/>
       <c r="T37" s="129"/>
@@ -2974,10 +3079,10 @@
       <c r="D38" s="149"/>
       <c r="E38" s="97"/>
       <c r="F38" s="133"/>
-      <c r="G38" s="26"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="97"/>
       <c r="I38" s="93"/>
-      <c r="J38" s="26"/>
+      <c r="J38" s="27"/>
       <c r="K38" s="97"/>
       <c r="L38" s="30"/>
       <c r="M38" s="90"/>
@@ -2993,7 +3098,7 @@
       <c r="X38" s="31"/>
     </row>
     <row r="39" spans="1:24">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B39" s="93"/>
@@ -3001,10 +3106,10 @@
       <c r="D39" s="149"/>
       <c r="E39" s="97"/>
       <c r="F39" s="133"/>
-      <c r="G39" s="26"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="97"/>
       <c r="I39" s="93"/>
-      <c r="J39" s="26"/>
+      <c r="J39" s="27"/>
       <c r="K39" s="97"/>
       <c r="L39" s="30"/>
       <c r="M39" s="90"/>
@@ -3020,7 +3125,7 @@
       <c r="X39" s="31"/>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B40" s="167"/>
@@ -3038,7 +3143,7 @@
       <c r="N40" s="36"/>
       <c r="O40" s="97"/>
       <c r="P40" s="136"/>
-      <c r="Q40" s="12"/>
+      <c r="Q40" s="13"/>
       <c r="R40" s="167"/>
       <c r="S40" s="97"/>
       <c r="T40" s="136"/>
@@ -3075,7 +3180,7 @@
       <c r="X41" s="38"/>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="58"/>
@@ -3093,7 +3198,7 @@
       <c r="N42" s="34"/>
       <c r="O42" s="97"/>
       <c r="P42" s="136"/>
-      <c r="Q42" s="14"/>
+      <c r="Q42" s="15"/>
       <c r="R42" s="59"/>
       <c r="S42" s="97"/>
       <c r="T42" s="136"/>
@@ -3108,10 +3213,10 @@
       <c r="D43" s="149"/>
       <c r="E43" s="97"/>
       <c r="F43" s="133"/>
-      <c r="G43" s="26"/>
+      <c r="G43" s="27"/>
       <c r="H43" s="97"/>
       <c r="I43" s="93"/>
-      <c r="J43" s="26"/>
+      <c r="J43" s="27"/>
       <c r="K43" s="97"/>
       <c r="L43" s="30"/>
       <c r="M43" s="90"/>
@@ -3154,7 +3259,7 @@
       <c r="X44" s="53"/>
     </row>
     <row r="45" spans="1:24" s="1" customFormat="1">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B45" s="170"/>
@@ -3164,7 +3269,7 @@
       </c>
       <c r="E45" s="99"/>
       <c r="F45" s="137"/>
-      <c r="G45" s="26" t="s">
+      <c r="G45" s="27" t="s">
         <v>63</v>
       </c>
       <c r="H45" s="99"/>
@@ -3176,19 +3281,19 @@
       <c r="N45" s="70"/>
       <c r="O45" s="99"/>
       <c r="P45" s="137"/>
-      <c r="Q45" s="17"/>
+      <c r="Q45" s="18"/>
       <c r="R45" s="170"/>
       <c r="S45" s="99"/>
       <c r="T45" s="137"/>
       <c r="U45" s="70"/>
       <c r="V45" s="99"/>
       <c r="W45" s="137"/>
-      <c r="X45" s="26" t="s">
-        <v>108</v>
+      <c r="X45" s="27" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="8"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="93"/>
       <c r="C46" s="109"/>
       <c r="D46" s="149"/>
@@ -3213,7 +3318,7 @@
       <c r="X46" s="31"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="170"/>
@@ -3231,7 +3336,7 @@
       <c r="N47" s="78"/>
       <c r="O47" s="97"/>
       <c r="P47" s="129"/>
-      <c r="Q47" s="12"/>
+      <c r="Q47" s="13"/>
       <c r="R47" s="171"/>
       <c r="S47" s="97"/>
       <c r="T47" s="129"/>
@@ -3241,7 +3346,7 @@
       <c r="X47" s="34"/>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B48" s="171"/>
@@ -3259,7 +3364,7 @@
       <c r="N48" s="78"/>
       <c r="O48" s="97"/>
       <c r="P48" s="129"/>
-      <c r="Q48" s="12"/>
+      <c r="Q48" s="13"/>
       <c r="R48" s="171"/>
       <c r="S48" s="97"/>
       <c r="T48" s="129"/>
@@ -3293,7 +3398,7 @@
       <c r="X49" s="31"/>
     </row>
     <row r="50" spans="1:24">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="171"/>
@@ -3311,7 +3416,7 @@
       <c r="N50" s="78"/>
       <c r="O50" s="97"/>
       <c r="P50" s="129"/>
-      <c r="Q50" s="12"/>
+      <c r="Q50" s="13"/>
       <c r="R50" s="171"/>
       <c r="S50" s="97"/>
       <c r="T50" s="129"/>
@@ -3325,7 +3430,7 @@
       </c>
     </row>
     <row r="51" spans="1:24">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="171"/>
@@ -3343,7 +3448,7 @@
       <c r="N51" s="78"/>
       <c r="O51" s="97"/>
       <c r="P51" s="135"/>
-      <c r="Q51" s="14"/>
+      <c r="Q51" s="15"/>
       <c r="R51" s="171"/>
       <c r="S51" s="97"/>
       <c r="T51" s="135"/>
@@ -3353,7 +3458,7 @@
       <c r="X51" s="36"/>
     </row>
     <row r="52" spans="1:24">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B52" s="171"/>
@@ -3371,7 +3476,7 @@
       <c r="N52" s="78"/>
       <c r="O52" s="97"/>
       <c r="P52" s="129"/>
-      <c r="Q52" s="12"/>
+      <c r="Q52" s="13"/>
       <c r="R52" s="171"/>
       <c r="S52" s="97"/>
       <c r="T52" s="129"/>
@@ -3384,25 +3489,26 @@
       <c r="A53" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="93"/>
-      <c r="C53" s="117"/>
-      <c r="D53" s="155"/>
+      <c r="B53" s="171"/>
+      <c r="C53" s="116"/>
+      <c r="D53" s="154"/>
       <c r="E53" s="97"/>
-      <c r="F53" s="131"/>
-      <c r="G53" s="38"/>
+      <c r="F53" s="135"/>
+      <c r="G53" s="36"/>
       <c r="H53" s="97"/>
-      <c r="I53" s="93"/>
-      <c r="J53" s="38"/>
+      <c r="I53" s="171"/>
+      <c r="J53" s="36"/>
       <c r="K53" s="97"/>
-      <c r="L53" s="30"/>
-      <c r="M53" s="90"/>
-      <c r="N53" s="31"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="171"/>
+      <c r="N53" s="78"/>
       <c r="O53" s="97"/>
-      <c r="P53" s="130"/>
-      <c r="R53" s="90"/>
+      <c r="P53" s="135"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="171"/>
       <c r="S53" s="97"/>
-      <c r="T53" s="130"/>
-      <c r="U53" s="31"/>
+      <c r="T53" s="135"/>
+      <c r="U53" s="70"/>
       <c r="V53" s="97"/>
       <c r="W53" s="129"/>
       <c r="X53" s="34"/>
@@ -3432,7 +3538,7 @@
       <c r="X54" s="31"/>
     </row>
     <row r="55" spans="1:24">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="93"/>
@@ -3459,7 +3565,7 @@
       <c r="X55" s="31"/>
     </row>
     <row r="56" spans="1:24">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B56" s="171"/>
@@ -3479,7 +3585,7 @@
       <c r="N56" s="78"/>
       <c r="O56" s="97"/>
       <c r="P56" s="135"/>
-      <c r="Q56" s="14"/>
+      <c r="Q56" s="15"/>
       <c r="R56" s="171"/>
       <c r="S56" s="97"/>
       <c r="T56" s="135"/>
@@ -3489,7 +3595,7 @@
       <c r="X56" s="36"/>
     </row>
     <row r="57" spans="1:24">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B57" s="171"/>
@@ -3507,7 +3613,7 @@
       <c r="N57" s="78"/>
       <c r="O57" s="97"/>
       <c r="P57" s="129"/>
-      <c r="Q57" s="12"/>
+      <c r="Q57" s="13"/>
       <c r="R57" s="171"/>
       <c r="S57" s="97"/>
       <c r="T57" s="129"/>
@@ -3517,7 +3623,7 @@
       <c r="X57" s="34"/>
     </row>
     <row r="58" spans="1:24">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B58" s="171"/>
@@ -3535,7 +3641,7 @@
       <c r="N58" s="78"/>
       <c r="O58" s="97"/>
       <c r="P58" s="129"/>
-      <c r="Q58" s="12"/>
+      <c r="Q58" s="13"/>
       <c r="R58" s="171"/>
       <c r="S58" s="97"/>
       <c r="T58" s="129"/>
@@ -3545,7 +3651,7 @@
       <c r="X58" s="34"/>
     </row>
     <row r="59" spans="1:24">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B59" s="171"/>
@@ -3563,7 +3669,7 @@
       <c r="N59" s="78"/>
       <c r="O59" s="97"/>
       <c r="P59" s="129"/>
-      <c r="Q59" s="12"/>
+      <c r="Q59" s="13"/>
       <c r="R59" s="171"/>
       <c r="S59" s="97"/>
       <c r="T59" s="129"/>
@@ -3659,7 +3765,7 @@
       </c>
     </row>
     <row r="62" spans="1:24">
-      <c r="A62" s="7">
+      <c r="A62" s="8">
         <v>10</v>
       </c>
       <c r="B62" s="172">
@@ -3701,7 +3807,7 @@
       <c r="P62" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q62" s="18">
+      <c r="Q62" s="19">
         <v>2149</v>
       </c>
       <c r="R62" s="181">
@@ -3711,7 +3817,7 @@
       <c r="T62" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U62" s="26" t="s">
+      <c r="U62" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V62" s="100"/>
@@ -3723,7 +3829,7 @@
       </c>
     </row>
     <row r="63" spans="1:24">
-      <c r="A63" s="7">
+      <c r="A63" s="8">
         <v>15</v>
       </c>
       <c r="B63" s="172">
@@ -3765,7 +3871,7 @@
       <c r="P63" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q63" s="18" t="s">
+      <c r="Q63" s="19" t="s">
         <v>17</v>
       </c>
       <c r="R63" s="181">
@@ -3775,7 +3881,7 @@
       <c r="T63" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U63" s="26" t="s">
+      <c r="U63" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V63" s="100"/>
@@ -3787,7 +3893,7 @@
       </c>
     </row>
     <row r="64" spans="1:24">
-      <c r="A64" s="7">
+      <c r="A64" s="8">
         <v>20</v>
       </c>
       <c r="B64" s="172" t="s">
@@ -3829,7 +3935,7 @@
       <c r="P64" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q64" s="18" t="s">
+      <c r="Q64" s="19" t="s">
         <v>17</v>
       </c>
       <c r="R64" s="181">
@@ -3839,7 +3945,7 @@
       <c r="T64" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U64" s="26" t="s">
+      <c r="U64" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V64" s="100"/>
@@ -3851,7 +3957,7 @@
       </c>
     </row>
     <row r="65" spans="1:24">
-      <c r="A65" s="7">
+      <c r="A65" s="8">
         <v>25</v>
       </c>
       <c r="B65" s="172">
@@ -3893,7 +3999,7 @@
       <c r="P65" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q65" s="18">
+      <c r="Q65" s="19">
         <v>4799</v>
       </c>
       <c r="R65" s="181">
@@ -3903,7 +4009,7 @@
       <c r="T65" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U65" s="26" t="s">
+      <c r="U65" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V65" s="100"/>
@@ -3915,7 +4021,7 @@
       </c>
     </row>
     <row r="66" spans="1:24">
-      <c r="A66" s="7">
+      <c r="A66" s="8">
         <v>30</v>
       </c>
       <c r="B66" s="172" t="s">
@@ -3957,7 +4063,7 @@
       <c r="P66" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q66" s="18" t="s">
+      <c r="Q66" s="19" t="s">
         <v>17</v>
       </c>
       <c r="R66" s="181">
@@ -3967,7 +4073,7 @@
       <c r="T66" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U66" s="26" t="s">
+      <c r="U66" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V66" s="100"/>
@@ -3979,7 +4085,7 @@
       </c>
     </row>
     <row r="67" spans="1:24">
-      <c r="A67" s="7">
+      <c r="A67" s="8">
         <v>50</v>
       </c>
       <c r="B67" s="172">
@@ -4021,7 +4127,7 @@
       <c r="P67" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q67" s="18">
+      <c r="Q67" s="19">
         <v>6999</v>
       </c>
       <c r="R67" s="181">
@@ -4031,7 +4137,7 @@
       <c r="T67" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U67" s="26" t="s">
+      <c r="U67" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V67" s="100"/>
@@ -4043,7 +4149,7 @@
       </c>
     </row>
     <row r="68" spans="1:24">
-      <c r="A68" s="7">
+      <c r="A68" s="8">
         <v>100</v>
       </c>
       <c r="B68" s="172">
@@ -4085,7 +4191,7 @@
       <c r="P68" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q68" s="18">
+      <c r="Q68" s="19">
         <v>9999</v>
       </c>
       <c r="R68" s="181">
@@ -4095,7 +4201,7 @@
       <c r="T68" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U68" s="26" t="s">
+      <c r="U68" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V68" s="100"/>
@@ -4107,7 +4213,7 @@
       </c>
     </row>
     <row r="69" spans="1:24">
-      <c r="A69" s="7">
+      <c r="A69" s="8">
         <v>250</v>
       </c>
       <c r="B69" s="172" t="s">
@@ -4149,7 +4255,7 @@
       <c r="P69" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q69" s="18" t="s">
+      <c r="Q69" s="19" t="s">
         <v>19</v>
       </c>
       <c r="R69" s="181">
@@ -4159,7 +4265,7 @@
       <c r="T69" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U69" s="26" t="s">
+      <c r="U69" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V69" s="100"/>
@@ -4171,7 +4277,7 @@
       </c>
     </row>
     <row r="70" spans="1:24">
-      <c r="A70" s="7">
+      <c r="A70" s="8">
         <v>500</v>
       </c>
       <c r="B70" s="172">
@@ -4213,7 +4319,7 @@
       <c r="P70" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q70" s="18" t="s">
+      <c r="Q70" s="19" t="s">
         <v>19</v>
       </c>
       <c r="R70" s="181" t="s">
@@ -4223,7 +4329,7 @@
       <c r="T70" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U70" s="26" t="s">
+      <c r="U70" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V70" s="100"/>
@@ -4235,7 +4341,7 @@
       </c>
     </row>
     <row r="71" spans="1:24">
-      <c r="A71" s="7">
+      <c r="A71" s="8">
         <v>2000</v>
       </c>
       <c r="B71" s="172">
@@ -4277,7 +4383,7 @@
       <c r="P71" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q71" s="18" t="s">
+      <c r="Q71" s="19" t="s">
         <v>19</v>
       </c>
       <c r="R71" s="181" t="s">
@@ -4287,7 +4393,7 @@
       <c r="T71" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U71" s="26" t="s">
+      <c r="U71" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V71" s="100"/>
@@ -4299,7 +4405,7 @@
       </c>
     </row>
     <row r="72" spans="1:24">
-      <c r="A72" s="7">
+      <c r="A72" s="8">
         <v>10000</v>
       </c>
       <c r="B72" s="172" t="s">
@@ -4341,7 +4447,7 @@
       <c r="P72" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="Q72" s="18" t="s">
+      <c r="Q72" s="19" t="s">
         <v>19</v>
       </c>
       <c r="R72" s="181" t="s">
@@ -4351,7 +4457,7 @@
       <c r="T72" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="U72" s="26" t="s">
+      <c r="U72" s="27" t="s">
         <v>80</v>
       </c>
       <c r="V72" s="100"/>
@@ -4363,7 +4469,7 @@
       </c>
     </row>
     <row r="73" spans="1:24">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B73" s="173" t="s">
@@ -4372,7 +4478,7 @@
       <c r="C73" s="123">
         <v>24000</v>
       </c>
-      <c r="D73" s="193" t="s">
+      <c r="D73" s="194" t="s">
         <v>17</v>
       </c>
       <c r="E73" s="101"/>
@@ -4458,11 +4564,12 @@
   <sortState ref="A24:A28">
     <sortCondition ref="A24:A28"/>
   </sortState>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="L16:N16"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="T16:U16"/>
     <mergeCell ref="W16:X16"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B16:D16"/>

</xml_diff>

<commit_message>
Testopia 2.5 funktioniert auch mit Bugzilla 4.4
</commit_message>
<xml_diff>
--- a/BTR Tools Evaluation.xlsx
+++ b/BTR Tools Evaluation.xlsx
@@ -400,9 +400,9 @@
       <t xml:space="preserve">
 • Verlinkung  von TestCases / TestRuns und Bugs lässt sich sehr gut einpflegen und nachverfolgen
 • Bedienung sehr intuitiv und klar strukturiert (mmN besser als JIRA)
-• Bugzilla befindet sich weiterhin in Entwicklung. Testopia 2.5 läuft zuverlässig nur auf Bugzilla 4.2. Ob an einer neuen Version für Bugzilla 4.4 oder dem demnächst releastem 5.0 gearbeitet wird, ist zZ nicht herauszufinden.
+• Bugzilla befindet sich weiterhin in Entwicklung. Testopia 2.5 läuft zuverlässig offiziell nur auf Bugzilla 4.2. Ob an einer neuen Version für Bugzilla 4.4 oder dem demnächst releastem 5.0 gearbeitet wird, ist zZ nicht herauszufinden.Eigene Tests ergaben aber (nach einigen Bugfixes [s.u.]), dass Testopia 2.5 auch auf Bugzilla 4.4 läuft.
 • Dokumentation für Einsteiger (Bugzilla &amp; Testopia) hilfreich (englisch)
-• Fehler in Testopia 2.5 in Verbindung mit Bugzilla 4.2 (https://bugzilla. mozilla.org/show_bug.cgi?id=931961)
+• Fehler in Testopia 2.5 in Verbindung mit Bugzilla 4.2 &amp; 4.4 (https://bugzilla. mozilla.org/show_bug.cgi?id=931961)
 • Fehler in Testopia 2.5 in Verbindung mit Bugzilla 4.4 (https://bugzilla. mozilla.org/show_bug.cgi?id=980234)</t>
     </r>
   </si>
@@ -1312,6 +1312,34 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1321,15 +1349,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1339,25 +1358,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1658,7 +1658,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10:D10"/>
+      <selection pane="topRight" activeCell="F10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
@@ -1668,8 +1668,8 @@
     <col min="3" max="3" width="14.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="5"/>
-    <col min="6" max="6" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="8" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="5" customWidth="1"/>
     <col min="9" max="10" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="5" customWidth="1"/>
@@ -1916,7 +1916,7 @@
       <c r="C5" s="110">
         <v>42038</v>
       </c>
-      <c r="D5" s="192">
+      <c r="D5" s="189">
         <v>41904</v>
       </c>
       <c r="E5" s="97"/>
@@ -1993,15 +1993,15 @@
         <v>Link</v>
       </c>
       <c r="K6" s="97"/>
-      <c r="L6" s="193" t="str">
+      <c r="L6" s="190" t="str">
         <f>HYPERLINK("http://www.practitest.com/","Link")</f>
         <v>Link</v>
       </c>
-      <c r="M6" s="193" t="str">
+      <c r="M6" s="190" t="str">
         <f>HYPERLINK("http://www.practitest.com/","Link")</f>
         <v>Link</v>
       </c>
-      <c r="N6" s="193" t="str">
+      <c r="N6" s="190" t="str">
         <f>HYPERLINK("http://www.practitest.com/","Link")</f>
         <v>Link</v>
       </c>
@@ -2023,16 +2023,16 @@
         <f>HYPERLINK("www.redmine.org","Link")</f>
         <v>Link</v>
       </c>
-      <c r="U6" s="203" t="str">
+      <c r="U6" s="197" t="str">
         <f>HYPERLINK("http://www.testlodge.com/","Link")</f>
         <v>Link</v>
       </c>
       <c r="V6" s="97"/>
-      <c r="W6" s="204" t="str">
+      <c r="W6" s="198" t="str">
         <f>HYPERLINK("http://trac.edgewall.org/","Link")</f>
         <v>Link</v>
       </c>
-      <c r="X6" s="203" t="str">
+      <c r="X6" s="197" t="str">
         <f>HYPERLINK("http://trac-hacks.org/wiki/TestManagerForTracPlugin","Link")</f>
         <v>Link</v>
       </c>
@@ -2112,16 +2112,16 @@
         <v>Link</v>
       </c>
       <c r="K8" s="97"/>
-      <c r="L8" s="193" t="str">
-        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
-        <v>Link</v>
-      </c>
-      <c r="M8" s="193" t="str">
-        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
-        <v>Link</v>
-      </c>
-      <c r="N8" s="193" t="str">
-        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+      <c r="L8" s="190" t="str">
+        <f t="shared" ref="L8:N9" si="0">HYPERLINK("http://support.practitest.com/","Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="M8" s="190" t="str">
+        <f t="shared" si="0"/>
+        <v>Link</v>
+      </c>
+      <c r="N8" s="190" t="str">
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="O8" s="97"/>
@@ -2142,16 +2142,16 @@
         <f>HYPERLINK("http://www.redmine.org/guide","Link")</f>
         <v>Link</v>
       </c>
-      <c r="U8" s="203" t="str">
+      <c r="U8" s="197" t="str">
         <f>HYPERLINK("https://help.testlodge.com/home","Link")</f>
         <v>Link</v>
       </c>
       <c r="V8" s="97"/>
-      <c r="W8" s="204" t="str">
+      <c r="W8" s="198" t="str">
         <f>HYPERLINK("http://trac.edgewall.org/wiki/TracGuide","Link")</f>
         <v>Link</v>
       </c>
-      <c r="X8" s="203" t="str">
+      <c r="X8" s="197" t="str">
         <f>HYPERLINK("http://trac-hacks.org/wiki/TestManagerForTracPlugin","Link")</f>
         <v>Link</v>
       </c>
@@ -2191,16 +2191,16 @@
         <v>Link</v>
       </c>
       <c r="K9" s="97"/>
-      <c r="L9" s="193" t="str">
-        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
-        <v>Link</v>
-      </c>
-      <c r="M9" s="193" t="str">
-        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
-        <v>Link</v>
-      </c>
-      <c r="N9" s="193" t="str">
-        <f>HYPERLINK("http://support.practitest.com/","Link")</f>
+      <c r="L9" s="190" t="str">
+        <f t="shared" si="0"/>
+        <v>Link</v>
+      </c>
+      <c r="M9" s="190" t="str">
+        <f t="shared" si="0"/>
+        <v>Link</v>
+      </c>
+      <c r="N9" s="190" t="str">
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="O9" s="97"/>
@@ -2221,41 +2221,41 @@
         <f>HYPERLINK("http://www.redmine.org/guide","Link")</f>
         <v>Link</v>
       </c>
-      <c r="U9" s="203" t="str">
+      <c r="U9" s="197" t="str">
         <f>HYPERLINK("https://help.testlodge.com/home","Link")</f>
         <v>Link</v>
       </c>
       <c r="V9" s="97"/>
-      <c r="W9" s="204" t="str">
+      <c r="W9" s="198" t="str">
         <f>HYPERLINK("http://trac.edgewall.org/wiki/TracGuide","Link")</f>
         <v>Link</v>
       </c>
-      <c r="X9" s="203" t="str">
+      <c r="X9" s="197" t="str">
         <f>HYPERLINK("http://trac-hacks.org/wiki/TestManagerForTracPlugin","Link")</f>
         <v>Link</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="12" customFormat="1" ht="359.25" customHeight="1">
+    <row r="10" spans="1:24" s="12" customFormat="1" ht="341.25" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="189" t="s">
+      <c r="B10" s="199" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="190"/>
-      <c r="D10" s="191"/>
+      <c r="C10" s="200"/>
+      <c r="D10" s="201"/>
       <c r="E10" s="98"/>
-      <c r="F10" s="189" t="s">
+      <c r="F10" s="199" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="191"/>
+      <c r="G10" s="201"/>
       <c r="H10" s="98"/>
-      <c r="I10" s="189" t="s">
+      <c r="I10" s="199" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="191"/>
+      <c r="J10" s="201"/>
       <c r="K10" s="98"/>
-      <c r="L10" s="193"/>
+      <c r="L10" s="190"/>
       <c r="M10" s="166"/>
       <c r="N10" s="29"/>
       <c r="O10" s="98"/>
@@ -2412,43 +2412,43 @@
       <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="195" t="s">
+      <c r="B16" s="202" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="196"/>
-      <c r="D16" s="197"/>
+      <c r="C16" s="203"/>
+      <c r="D16" s="204"/>
       <c r="E16" s="97"/>
-      <c r="F16" s="195" t="s">
+      <c r="F16" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="197"/>
+      <c r="G16" s="204"/>
       <c r="H16" s="97"/>
-      <c r="I16" s="195" t="s">
+      <c r="I16" s="202" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="197"/>
+      <c r="J16" s="204"/>
       <c r="K16" s="97"/>
-      <c r="L16" s="195" t="s">
+      <c r="L16" s="202" t="s">
         <v>69</v>
       </c>
-      <c r="M16" s="196"/>
-      <c r="N16" s="197"/>
+      <c r="M16" s="203"/>
+      <c r="N16" s="204"/>
       <c r="O16" s="97"/>
-      <c r="P16" s="195" t="s">
+      <c r="P16" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="Q16" s="196"/>
-      <c r="R16" s="197"/>
+      <c r="Q16" s="203"/>
+      <c r="R16" s="204"/>
       <c r="S16" s="97"/>
-      <c r="T16" s="195" t="s">
+      <c r="T16" s="202" t="s">
         <v>81</v>
       </c>
-      <c r="U16" s="197"/>
+      <c r="U16" s="204"/>
       <c r="V16" s="97"/>
-      <c r="W16" s="195" t="s">
+      <c r="W16" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="X16" s="197"/>
+      <c r="X16" s="204"/>
     </row>
     <row r="17" spans="1:24">
       <c r="B17" s="90"/>
@@ -2868,74 +2868,74 @@
       <c r="A29" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="198" t="str">
+      <c r="B29" s="192" t="str">
         <f>HYPERLINK("https://docs.atlassian.com/jira/REST/latest/","REST")</f>
         <v>REST</v>
       </c>
-      <c r="C29" s="199" t="str">
+      <c r="C29" s="193" t="str">
         <f>HYPERLINK("https://docs.atlassian.com/jira/REST/latest/","REST")</f>
         <v>REST</v>
       </c>
       <c r="D29" s="156"/>
       <c r="E29" s="99"/>
-      <c r="F29" s="200" t="str">
+      <c r="F29" s="194" t="str">
         <f>HYPERLINK("https://wiki.mozilla.org/Bugzilla:REST_API","REST")</f>
         <v>REST</v>
       </c>
-      <c r="G29" s="201" t="str">
+      <c r="G29" s="195" t="str">
         <f>HYPERLINK("https://wiki.mozilla.org/Testopia:Documentation","XMLRPC")</f>
         <v>XMLRPC</v>
       </c>
       <c r="H29" s="99"/>
-      <c r="I29" s="198" t="str">
+      <c r="I29" s="192" t="str">
         <f>HYPERLINK("http://www.inflectra.com/SpiraDemo/Services/v4_0/RestService.aspx","REST")</f>
         <v>REST</v>
       </c>
-      <c r="J29" s="198" t="str">
+      <c r="J29" s="192" t="str">
         <f>HYPERLINK("http://www.inflectra.com/SpiraDemo/Services/v4_0/RestService.aspx","REST")</f>
         <v>REST</v>
       </c>
       <c r="K29" s="99"/>
-      <c r="L29" s="201" t="str">
+      <c r="L29" s="195" t="str">
         <f>HYPERLINK("http://support.practitest.com/customer/portal/topics/394423-api/articles","REST")</f>
         <v>REST</v>
       </c>
-      <c r="M29" s="201" t="str">
+      <c r="M29" s="195" t="str">
         <f>HYPERLINK("http://support.practitest.com/customer/portal/topics/394423-api/articles","REST")</f>
         <v>REST</v>
       </c>
-      <c r="N29" s="201" t="str">
+      <c r="N29" s="195" t="str">
         <f>HYPERLINK("http://support.practitest.com/customer/portal/topics/394423-api/articles","REST")</f>
         <v>REST</v>
       </c>
       <c r="O29" s="99"/>
-      <c r="P29" s="200" t="str">
+      <c r="P29" s="194" t="str">
         <f>HYPERLINK("http://mantishub.readthedocs.org/api.html","SOAP")</f>
         <v>SOAP</v>
       </c>
-      <c r="Q29" s="202" t="str">
+      <c r="Q29" s="196" t="str">
         <f>HYPERLINK("http://docs.gurock.com/testrail-api2/start","API")</f>
         <v>API</v>
       </c>
-      <c r="R29" s="198" t="str">
+      <c r="R29" s="192" t="str">
         <f>HYPERLINK("http://docs.gurock.com/testrail-api2/start","API")</f>
         <v>API</v>
       </c>
       <c r="S29" s="99"/>
-      <c r="T29" s="200" t="str">
+      <c r="T29" s="194" t="str">
         <f>HYPERLINK("http://www.redmine.org/projects/redmine/wiki/Rest_api","REST")</f>
         <v>REST</v>
       </c>
-      <c r="U29" s="201" t="str">
+      <c r="U29" s="195" t="str">
         <f>HYPERLINK("https://help.testlodge.com/categories/20144806-TestLodge-API","REST")</f>
         <v>REST</v>
       </c>
       <c r="V29" s="99"/>
-      <c r="W29" s="200" t="str">
+      <c r="W29" s="194" t="str">
         <f>HYPERLINK("http://trac.edgewall.org/wiki/TracDev/ApiDocs","API")</f>
         <v>API</v>
       </c>
-      <c r="X29" s="201" t="str">
+      <c r="X29" s="195" t="str">
         <f>HYPERLINK("http://trac-hacks.org/wiki/TestManagerForTracPlugin","REST / XMLRPC")</f>
         <v>REST / XMLRPC</v>
       </c>
@@ -3885,11 +3885,11 @@
         <v>150</v>
       </c>
       <c r="M62" s="172">
-        <f t="shared" ref="M62:M72" si="0">A62*35</f>
+        <f t="shared" ref="M62:M72" si="1">A62*35</f>
         <v>350</v>
       </c>
       <c r="N62" s="43">
-        <f t="shared" ref="N62:N72" si="1">A62*45</f>
+        <f t="shared" ref="N62:N72" si="2">A62*45</f>
         <v>450</v>
       </c>
       <c r="O62" s="100"/>
@@ -3949,11 +3949,11 @@
         <v>225</v>
       </c>
       <c r="M63" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>525</v>
       </c>
       <c r="N63" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>675</v>
       </c>
       <c r="O63" s="100"/>
@@ -4013,11 +4013,11 @@
         <v>300</v>
       </c>
       <c r="M64" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>700</v>
       </c>
       <c r="N64" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>900</v>
       </c>
       <c r="O64" s="100"/>
@@ -4077,11 +4077,11 @@
         <v>375</v>
       </c>
       <c r="M65" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>875</v>
       </c>
       <c r="N65" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1125</v>
       </c>
       <c r="O65" s="100"/>
@@ -4141,11 +4141,11 @@
         <v>450</v>
       </c>
       <c r="M66" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1050</v>
       </c>
       <c r="N66" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1350</v>
       </c>
       <c r="O66" s="100"/>
@@ -4205,11 +4205,11 @@
         <v>750</v>
       </c>
       <c r="M67" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1750</v>
       </c>
       <c r="N67" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2250</v>
       </c>
       <c r="O67" s="100"/>
@@ -4269,11 +4269,11 @@
         <v>1500</v>
       </c>
       <c r="M68" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3500</v>
       </c>
       <c r="N68" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4500</v>
       </c>
       <c r="O68" s="100"/>
@@ -4333,11 +4333,11 @@
         <v>3750</v>
       </c>
       <c r="M69" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8750</v>
       </c>
       <c r="N69" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11250</v>
       </c>
       <c r="O69" s="100"/>
@@ -4397,11 +4397,11 @@
         <v>7500</v>
       </c>
       <c r="M70" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17500</v>
       </c>
       <c r="N70" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22500</v>
       </c>
       <c r="O70" s="100"/>
@@ -4461,11 +4461,11 @@
         <v>30000</v>
       </c>
       <c r="M71" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="N71" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90000</v>
       </c>
       <c r="O71" s="100"/>
@@ -4525,11 +4525,11 @@
         <v>150000</v>
       </c>
       <c r="M72" s="172">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>350000</v>
       </c>
       <c r="N72" s="43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>450000</v>
       </c>
       <c r="O72" s="100"/>
@@ -4567,7 +4567,7 @@
       <c r="C73" s="123">
         <v>24000</v>
       </c>
-      <c r="D73" s="194" t="s">
+      <c r="D73" s="191" t="s">
         <v>17</v>
       </c>
       <c r="E73" s="101"/>

</xml_diff>

<commit_message>
Trennung Migration & Integration
Trennung Migration & Integration zum besseren Verständnis
</commit_message>
<xml_diff>
--- a/BTR Tools Evaluation.xlsx
+++ b/BTR Tools Evaluation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="111">
   <si>
     <t>Fehlermanagement</t>
   </si>
@@ -404,7 +404,10 @@
     </r>
   </si>
   <si>
-    <t>Bugtracker (Migration)</t>
+    <t>Bugtracker Integration</t>
+  </si>
+  <si>
+    <t>Bugtracker Migration von …</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +551,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -882,7 +891,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1338,24 +1347,31 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1651,12 +1667,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X79"/>
+  <dimension ref="A1:X87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="topRight" activeCell="F34" sqref="F34"/>
+      <selection pane="topRight" activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
@@ -2237,21 +2253,21 @@
       <c r="A10" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="200" t="s">
+      <c r="B10" s="197" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="202"/>
-      <c r="D10" s="201"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="199"/>
       <c r="E10" s="98"/>
-      <c r="F10" s="200" t="s">
+      <c r="F10" s="197" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="201"/>
+      <c r="G10" s="199"/>
       <c r="H10" s="98"/>
-      <c r="I10" s="200" t="s">
+      <c r="I10" s="197" t="s">
         <v>105</v>
       </c>
-      <c r="J10" s="201"/>
+      <c r="J10" s="199"/>
       <c r="K10" s="98"/>
       <c r="L10" s="189"/>
       <c r="M10" s="165"/>
@@ -2410,43 +2426,43 @@
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="197" t="s">
+      <c r="B16" s="200" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="198"/>
-      <c r="D16" s="199"/>
+      <c r="C16" s="201"/>
+      <c r="D16" s="202"/>
       <c r="E16" s="97"/>
-      <c r="F16" s="197" t="s">
+      <c r="F16" s="200" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="199"/>
+      <c r="G16" s="202"/>
       <c r="H16" s="97"/>
-      <c r="I16" s="197" t="s">
+      <c r="I16" s="200" t="s">
         <v>70</v>
       </c>
-      <c r="J16" s="199"/>
+      <c r="J16" s="202"/>
       <c r="K16" s="97"/>
-      <c r="L16" s="197" t="s">
+      <c r="L16" s="200" t="s">
         <v>68</v>
       </c>
-      <c r="M16" s="198"/>
-      <c r="N16" s="199"/>
+      <c r="M16" s="201"/>
+      <c r="N16" s="202"/>
       <c r="O16" s="97"/>
-      <c r="P16" s="197" t="s">
+      <c r="P16" s="200" t="s">
         <v>69</v>
       </c>
-      <c r="Q16" s="198"/>
-      <c r="R16" s="199"/>
+      <c r="Q16" s="201"/>
+      <c r="R16" s="202"/>
       <c r="S16" s="97"/>
-      <c r="T16" s="197" t="s">
+      <c r="T16" s="200" t="s">
         <v>80</v>
       </c>
-      <c r="U16" s="199"/>
+      <c r="U16" s="202"/>
       <c r="V16" s="97"/>
-      <c r="W16" s="197" t="s">
+      <c r="W16" s="200" t="s">
         <v>69</v>
       </c>
-      <c r="X16" s="199"/>
+      <c r="X16" s="202"/>
     </row>
     <row r="17" spans="1:24">
       <c r="B17" s="90"/>
@@ -2964,7 +2980,7 @@
       <c r="X30" s="31"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B31" s="90"/>
@@ -2994,11 +3010,11 @@
       <c r="A32" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="166"/>
-      <c r="C32" s="112"/>
+      <c r="B32" s="204"/>
+      <c r="C32" s="207"/>
       <c r="D32" s="153"/>
       <c r="E32" s="97"/>
-      <c r="F32" s="129"/>
+      <c r="F32" s="208"/>
       <c r="G32" s="34"/>
       <c r="H32" s="97"/>
       <c r="I32" s="166"/>
@@ -3008,25 +3024,25 @@
       <c r="M32" s="166"/>
       <c r="N32" s="34"/>
       <c r="O32" s="97"/>
-      <c r="P32" s="135"/>
+      <c r="P32" s="208"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="166"/>
       <c r="S32" s="97"/>
-      <c r="T32" s="129"/>
+      <c r="T32" s="208"/>
       <c r="U32" s="34"/>
       <c r="V32" s="97"/>
-      <c r="W32" s="136"/>
-      <c r="X32" s="88"/>
+      <c r="W32" s="130"/>
+      <c r="X32" s="31"/>
     </row>
     <row r="33" spans="1:24">
       <c r="A33" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="166"/>
-      <c r="C33" s="112"/>
+      <c r="B33" s="204"/>
+      <c r="C33" s="207"/>
       <c r="D33" s="153"/>
       <c r="E33" s="97"/>
-      <c r="F33" s="135"/>
+      <c r="F33" s="208"/>
       <c r="G33" s="36"/>
       <c r="H33" s="97"/>
       <c r="I33" s="59"/>
@@ -3036,27 +3052,25 @@
       <c r="M33" s="59"/>
       <c r="N33" s="36"/>
       <c r="O33" s="97"/>
-      <c r="P33" s="135"/>
+      <c r="P33" s="208"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="59"/>
       <c r="S33" s="97"/>
-      <c r="T33" s="135"/>
+      <c r="T33" s="208"/>
       <c r="U33" s="36"/>
       <c r="V33" s="97"/>
-      <c r="W33" s="135"/>
-      <c r="X33" s="88"/>
+      <c r="W33" s="130"/>
+      <c r="X33" s="31"/>
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="166"/>
-      <c r="C34" s="112"/>
+      <c r="B34" s="204"/>
+      <c r="C34" s="207"/>
       <c r="D34" s="151"/>
       <c r="E34" s="97"/>
-      <c r="F34" s="136" t="s">
-        <v>63</v>
-      </c>
+      <c r="F34" s="208"/>
       <c r="G34" s="36"/>
       <c r="H34" s="97"/>
       <c r="I34" s="166"/>
@@ -3066,25 +3080,25 @@
       <c r="M34" s="166"/>
       <c r="N34" s="34"/>
       <c r="O34" s="97"/>
-      <c r="P34" s="135"/>
+      <c r="P34" s="208"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="166"/>
       <c r="S34" s="97"/>
-      <c r="T34" s="129"/>
+      <c r="T34" s="208"/>
       <c r="U34" s="34"/>
       <c r="V34" s="97"/>
-      <c r="W34" s="136"/>
-      <c r="X34" s="88"/>
+      <c r="W34" s="130"/>
+      <c r="X34" s="31"/>
     </row>
     <row r="35" spans="1:24">
       <c r="A35" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="166"/>
-      <c r="C35" s="112"/>
+      <c r="B35" s="204"/>
+      <c r="C35" s="207"/>
       <c r="D35" s="153"/>
       <c r="E35" s="97"/>
-      <c r="F35" s="135"/>
+      <c r="F35" s="208"/>
       <c r="G35" s="36"/>
       <c r="H35" s="97"/>
       <c r="I35" s="166"/>
@@ -3094,25 +3108,25 @@
       <c r="M35" s="59"/>
       <c r="N35" s="36"/>
       <c r="O35" s="97"/>
-      <c r="P35" s="135"/>
+      <c r="P35" s="208"/>
       <c r="Q35" s="13"/>
       <c r="R35" s="166"/>
       <c r="S35" s="97"/>
-      <c r="T35" s="129"/>
+      <c r="T35" s="208"/>
       <c r="U35" s="34"/>
       <c r="V35" s="97"/>
-      <c r="W35" s="136"/>
-      <c r="X35" s="88"/>
+      <c r="W35" s="130"/>
+      <c r="X35" s="31"/>
     </row>
     <row r="36" spans="1:24">
       <c r="A36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="166"/>
-      <c r="C36" s="112"/>
+      <c r="B36" s="204"/>
+      <c r="C36" s="207"/>
       <c r="D36" s="153"/>
       <c r="E36" s="97"/>
-      <c r="F36" s="135"/>
+      <c r="F36" s="208"/>
       <c r="G36" s="36"/>
       <c r="H36" s="97"/>
       <c r="I36" s="166"/>
@@ -3122,25 +3136,25 @@
       <c r="M36" s="166"/>
       <c r="N36" s="34"/>
       <c r="O36" s="97"/>
-      <c r="P36" s="135"/>
+      <c r="P36" s="208"/>
       <c r="Q36" s="13"/>
       <c r="R36" s="166"/>
       <c r="S36" s="97"/>
-      <c r="T36" s="129"/>
+      <c r="T36" s="208"/>
       <c r="U36" s="34"/>
       <c r="V36" s="97"/>
-      <c r="W36" s="135"/>
-      <c r="X36" s="88"/>
+      <c r="W36" s="130"/>
+      <c r="X36" s="31"/>
     </row>
     <row r="37" spans="1:24">
       <c r="A37" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="166"/>
-      <c r="C37" s="112"/>
+      <c r="B37" s="204"/>
+      <c r="C37" s="207"/>
       <c r="D37" s="153"/>
       <c r="E37" s="97"/>
-      <c r="F37" s="135"/>
+      <c r="F37" s="208"/>
       <c r="G37" s="36"/>
       <c r="H37" s="97"/>
       <c r="I37" s="59"/>
@@ -3150,30 +3164,30 @@
       <c r="M37" s="59"/>
       <c r="N37" s="36"/>
       <c r="O37" s="97"/>
-      <c r="P37" s="135"/>
+      <c r="P37" s="208"/>
       <c r="Q37" s="13"/>
       <c r="R37" s="166"/>
       <c r="S37" s="97"/>
-      <c r="T37" s="129"/>
+      <c r="T37" s="208"/>
       <c r="U37" s="36"/>
       <c r="V37" s="97"/>
-      <c r="W37" s="129"/>
-      <c r="X37" s="34"/>
+      <c r="W37" s="130"/>
+      <c r="X37" s="31"/>
     </row>
     <row r="38" spans="1:24">
-      <c r="B38" s="93"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="148"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="152"/>
       <c r="E38" s="97"/>
-      <c r="F38" s="133"/>
-      <c r="G38" s="27"/>
+      <c r="F38" s="130"/>
+      <c r="G38" s="31"/>
       <c r="H38" s="97"/>
-      <c r="I38" s="93"/>
-      <c r="J38" s="27"/>
+      <c r="I38" s="90"/>
+      <c r="J38" s="31"/>
       <c r="K38" s="97"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="90"/>
-      <c r="N38" s="31"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="179"/>
+      <c r="N38" s="77"/>
       <c r="O38" s="97"/>
       <c r="P38" s="130"/>
       <c r="R38" s="90"/>
@@ -3186,21 +3200,21 @@
     </row>
     <row r="39" spans="1:24">
       <c r="A39" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="109"/>
-      <c r="D39" s="148"/>
+        <v>110</v>
+      </c>
+      <c r="B39" s="90"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="152"/>
       <c r="E39" s="97"/>
-      <c r="F39" s="133"/>
-      <c r="G39" s="27"/>
+      <c r="F39" s="130"/>
+      <c r="G39" s="31"/>
       <c r="H39" s="97"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="27"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="31"/>
       <c r="K39" s="97"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="90"/>
-      <c r="N39" s="31"/>
+      <c r="L39" s="76"/>
+      <c r="M39" s="179"/>
+      <c r="N39" s="77"/>
       <c r="O39" s="97"/>
       <c r="P39" s="130"/>
       <c r="R39" s="90"/>
@@ -3213,183 +3227,184 @@
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B40" s="166"/>
       <c r="C40" s="112"/>
-      <c r="D40" s="150"/>
+      <c r="D40" s="206"/>
       <c r="E40" s="97"/>
-      <c r="F40" s="136"/>
-      <c r="G40" s="33"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="205"/>
       <c r="H40" s="97"/>
-      <c r="I40" s="175"/>
-      <c r="J40" s="69"/>
+      <c r="I40" s="204"/>
+      <c r="J40" s="205"/>
       <c r="K40" s="97"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="36"/>
+      <c r="L40" s="203"/>
+      <c r="M40" s="204"/>
+      <c r="N40" s="205"/>
       <c r="O40" s="97"/>
-      <c r="P40" s="136"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="166"/>
+      <c r="P40" s="135"/>
+      <c r="Q40" s="209"/>
+      <c r="R40" s="204"/>
       <c r="S40" s="97"/>
-      <c r="T40" s="136"/>
-      <c r="U40" s="34"/>
+      <c r="T40" s="135"/>
+      <c r="U40" s="205"/>
       <c r="V40" s="97"/>
-      <c r="W40" s="129"/>
+      <c r="W40" s="136"/>
       <c r="X40" s="88"/>
     </row>
-    <row r="41" spans="1:24" s="5" customFormat="1">
+    <row r="41" spans="1:24">
       <c r="A41" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="117"/>
-      <c r="D41" s="154"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="144"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="89"/>
-      <c r="I41" s="94"/>
-      <c r="J41" s="80"/>
-      <c r="K41" s="89"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="89"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="89"/>
-      <c r="P41" s="144"/>
-      <c r="R41" s="89"/>
-      <c r="S41" s="89"/>
-      <c r="T41" s="144"/>
-      <c r="U41" s="38"/>
-      <c r="V41" s="89"/>
-      <c r="W41" s="131"/>
-      <c r="X41" s="38"/>
+        <v>46</v>
+      </c>
+      <c r="B41" s="166"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="206"/>
+      <c r="E41" s="97"/>
+      <c r="F41" s="135"/>
+      <c r="G41" s="205"/>
+      <c r="H41" s="97"/>
+      <c r="I41" s="204"/>
+      <c r="J41" s="205"/>
+      <c r="K41" s="97"/>
+      <c r="L41" s="203"/>
+      <c r="M41" s="204"/>
+      <c r="N41" s="205"/>
+      <c r="O41" s="97"/>
+      <c r="P41" s="135"/>
+      <c r="Q41" s="209"/>
+      <c r="R41" s="204"/>
+      <c r="S41" s="97"/>
+      <c r="T41" s="135"/>
+      <c r="U41" s="205"/>
+      <c r="V41" s="97"/>
+      <c r="W41" s="135"/>
+      <c r="X41" s="88"/>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="58"/>
-      <c r="C42" s="113"/>
-      <c r="D42" s="150"/>
+      <c r="A42" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="166"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="206"/>
       <c r="E42" s="97"/>
-      <c r="F42" s="136"/>
-      <c r="G42" s="33"/>
+      <c r="F42" s="136" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" s="205"/>
       <c r="H42" s="97"/>
-      <c r="I42" s="175"/>
-      <c r="J42" s="69"/>
+      <c r="I42" s="204"/>
+      <c r="J42" s="205"/>
       <c r="K42" s="97"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="166"/>
-      <c r="N42" s="34"/>
+      <c r="L42" s="203"/>
+      <c r="M42" s="204"/>
+      <c r="N42" s="205"/>
       <c r="O42" s="97"/>
-      <c r="P42" s="136"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="59"/>
+      <c r="P42" s="135"/>
+      <c r="Q42" s="209"/>
+      <c r="R42" s="204"/>
       <c r="S42" s="97"/>
-      <c r="T42" s="136"/>
-      <c r="U42" s="36"/>
+      <c r="T42" s="135"/>
+      <c r="U42" s="205"/>
       <c r="V42" s="97"/>
-      <c r="W42" s="129"/>
+      <c r="W42" s="136"/>
       <c r="X42" s="88"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="B43" s="93"/>
-      <c r="C43" s="109"/>
-      <c r="D43" s="148"/>
+      <c r="A43" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="166"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="206"/>
       <c r="E43" s="97"/>
-      <c r="F43" s="133"/>
-      <c r="G43" s="27"/>
+      <c r="F43" s="135"/>
+      <c r="G43" s="205"/>
       <c r="H43" s="97"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="27"/>
+      <c r="I43" s="204"/>
+      <c r="J43" s="205"/>
       <c r="K43" s="97"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="90"/>
-      <c r="N43" s="31"/>
+      <c r="L43" s="203"/>
+      <c r="M43" s="204"/>
+      <c r="N43" s="205"/>
       <c r="O43" s="97"/>
-      <c r="P43" s="130"/>
-      <c r="R43" s="90"/>
+      <c r="P43" s="129"/>
+      <c r="Q43" s="209"/>
+      <c r="R43" s="204"/>
       <c r="S43" s="97"/>
-      <c r="T43" s="130"/>
-      <c r="U43" s="31"/>
+      <c r="T43" s="135"/>
+      <c r="U43" s="205"/>
       <c r="V43" s="97"/>
-      <c r="W43" s="130"/>
-      <c r="X43" s="31"/>
-    </row>
-    <row r="44" spans="1:24" s="52" customFormat="1">
-      <c r="A44" s="162" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="168"/>
-      <c r="C44" s="119"/>
-      <c r="D44" s="157"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="134"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="48"/>
-      <c r="P44" s="134"/>
-      <c r="R44" s="48"/>
-      <c r="S44" s="48"/>
-      <c r="T44" s="134"/>
-      <c r="U44" s="53"/>
-      <c r="V44" s="48"/>
-      <c r="W44" s="134"/>
-      <c r="X44" s="53"/>
-    </row>
-    <row r="45" spans="1:24" s="1" customFormat="1">
-      <c r="A45" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="169"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="148" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="99"/>
-      <c r="F45" s="137"/>
-      <c r="G45" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="H45" s="99"/>
-      <c r="I45" s="169"/>
-      <c r="J45" s="70"/>
-      <c r="K45" s="99"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="169"/>
-      <c r="N45" s="70"/>
-      <c r="O45" s="99"/>
-      <c r="P45" s="137"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="169"/>
-      <c r="S45" s="99"/>
-      <c r="T45" s="137"/>
-      <c r="U45" s="70"/>
-      <c r="V45" s="99"/>
-      <c r="W45" s="137"/>
-      <c r="X45" s="27" t="s">
-        <v>104</v>
-      </c>
+      <c r="W43" s="136"/>
+      <c r="X43" s="88"/>
+    </row>
+    <row r="44" spans="1:24">
+      <c r="A44" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="166"/>
+      <c r="C44" s="112"/>
+      <c r="D44" s="206"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="135"/>
+      <c r="G44" s="205"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="204"/>
+      <c r="J44" s="205"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="203"/>
+      <c r="M44" s="204"/>
+      <c r="N44" s="205"/>
+      <c r="O44" s="97"/>
+      <c r="P44" s="135"/>
+      <c r="Q44" s="209"/>
+      <c r="R44" s="204"/>
+      <c r="S44" s="97"/>
+      <c r="T44" s="129"/>
+      <c r="U44" s="205"/>
+      <c r="V44" s="97"/>
+      <c r="W44" s="135"/>
+      <c r="X44" s="88"/>
+    </row>
+    <row r="45" spans="1:24">
+      <c r="A45" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="166"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="206"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="135"/>
+      <c r="G45" s="205"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="204"/>
+      <c r="J45" s="205"/>
+      <c r="K45" s="97"/>
+      <c r="L45" s="203"/>
+      <c r="M45" s="204"/>
+      <c r="N45" s="205"/>
+      <c r="O45" s="97"/>
+      <c r="P45" s="135"/>
+      <c r="Q45" s="209"/>
+      <c r="R45" s="204"/>
+      <c r="S45" s="97"/>
+      <c r="T45" s="135"/>
+      <c r="U45" s="205"/>
+      <c r="V45" s="97"/>
+      <c r="W45" s="129"/>
+      <c r="X45" s="34"/>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="9"/>
       <c r="B46" s="93"/>
       <c r="C46" s="109"/>
       <c r="D46" s="148"/>
       <c r="E46" s="97"/>
-      <c r="F46" s="130"/>
-      <c r="G46" s="31"/>
+      <c r="F46" s="133"/>
+      <c r="G46" s="27"/>
       <c r="H46" s="97"/>
       <c r="I46" s="93"/>
-      <c r="J46" s="31"/>
+      <c r="J46" s="27"/>
       <c r="K46" s="97"/>
       <c r="L46" s="30"/>
       <c r="M46" s="90"/>
@@ -3405,211 +3420,211 @@
       <c r="X46" s="31"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="A47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="169"/>
-      <c r="C47" s="112"/>
-      <c r="D47" s="151"/>
+      <c r="A47" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="93"/>
+      <c r="C47" s="109"/>
+      <c r="D47" s="148"/>
       <c r="E47" s="97"/>
-      <c r="F47" s="129"/>
-      <c r="G47" s="34"/>
+      <c r="F47" s="133"/>
+      <c r="G47" s="27"/>
       <c r="H47" s="97"/>
-      <c r="I47" s="170"/>
-      <c r="J47" s="36"/>
+      <c r="I47" s="93"/>
+      <c r="J47" s="27"/>
       <c r="K47" s="97"/>
-      <c r="L47" s="41"/>
-      <c r="M47" s="170"/>
-      <c r="N47" s="78"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="90"/>
+      <c r="N47" s="31"/>
       <c r="O47" s="97"/>
-      <c r="P47" s="129"/>
-      <c r="Q47" s="13"/>
-      <c r="R47" s="170"/>
+      <c r="P47" s="130"/>
+      <c r="R47" s="90"/>
       <c r="S47" s="97"/>
-      <c r="T47" s="129"/>
-      <c r="U47" s="70"/>
+      <c r="T47" s="130"/>
+      <c r="U47" s="31"/>
       <c r="V47" s="97"/>
-      <c r="W47" s="129"/>
-      <c r="X47" s="34"/>
+      <c r="W47" s="130"/>
+      <c r="X47" s="31"/>
     </row>
     <row r="48" spans="1:24">
       <c r="A48" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="170"/>
+        <v>53</v>
+      </c>
+      <c r="B48" s="166"/>
       <c r="C48" s="112"/>
-      <c r="D48" s="151"/>
+      <c r="D48" s="150"/>
       <c r="E48" s="97"/>
-      <c r="F48" s="129"/>
-      <c r="G48" s="34"/>
+      <c r="F48" s="136"/>
+      <c r="G48" s="33"/>
       <c r="H48" s="97"/>
-      <c r="I48" s="170"/>
-      <c r="J48" s="34"/>
+      <c r="I48" s="175"/>
+      <c r="J48" s="69"/>
       <c r="K48" s="97"/>
-      <c r="L48" s="41"/>
-      <c r="M48" s="170"/>
-      <c r="N48" s="78"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="59"/>
+      <c r="N48" s="36"/>
       <c r="O48" s="97"/>
-      <c r="P48" s="129"/>
+      <c r="P48" s="136"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="170"/>
+      <c r="R48" s="166"/>
       <c r="S48" s="97"/>
-      <c r="T48" s="129"/>
-      <c r="U48" s="70"/>
+      <c r="T48" s="136"/>
+      <c r="U48" s="34"/>
       <c r="V48" s="97"/>
       <c r="W48" s="129"/>
-      <c r="X48" s="34"/>
-    </row>
-    <row r="49" spans="1:24">
-      <c r="B49" s="93"/>
+      <c r="X48" s="88"/>
+    </row>
+    <row r="49" spans="1:24" s="5" customFormat="1">
+      <c r="A49" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="89"/>
       <c r="C49" s="117"/>
       <c r="D49" s="154"/>
-      <c r="E49" s="97"/>
-      <c r="F49" s="131"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="144"/>
       <c r="G49" s="38"/>
-      <c r="H49" s="97"/>
-      <c r="I49" s="93"/>
-      <c r="J49" s="38"/>
-      <c r="K49" s="97"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="90"/>
-      <c r="N49" s="31"/>
-      <c r="O49" s="97"/>
-      <c r="P49" s="130"/>
-      <c r="R49" s="90"/>
-      <c r="S49" s="97"/>
-      <c r="T49" s="130"/>
-      <c r="U49" s="31"/>
-      <c r="V49" s="97"/>
-      <c r="W49" s="130"/>
-      <c r="X49" s="31"/>
+      <c r="H49" s="89"/>
+      <c r="I49" s="94"/>
+      <c r="J49" s="80"/>
+      <c r="K49" s="89"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="89"/>
+      <c r="N49" s="38"/>
+      <c r="O49" s="89"/>
+      <c r="P49" s="144"/>
+      <c r="R49" s="89"/>
+      <c r="S49" s="89"/>
+      <c r="T49" s="144"/>
+      <c r="U49" s="38"/>
+      <c r="V49" s="89"/>
+      <c r="W49" s="131"/>
+      <c r="X49" s="38"/>
     </row>
     <row r="50" spans="1:24">
       <c r="A50" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" s="170"/>
-      <c r="C50" s="116"/>
-      <c r="D50" s="153"/>
+        <v>48</v>
+      </c>
+      <c r="B50" s="58"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="150"/>
       <c r="E50" s="97"/>
-      <c r="F50" s="129"/>
-      <c r="G50" s="34"/>
+      <c r="F50" s="136"/>
+      <c r="G50" s="33"/>
       <c r="H50" s="97"/>
-      <c r="I50" s="170"/>
-      <c r="J50" s="36"/>
+      <c r="I50" s="175"/>
+      <c r="J50" s="69"/>
       <c r="K50" s="97"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="170"/>
-      <c r="N50" s="78"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="166"/>
+      <c r="N50" s="34"/>
       <c r="O50" s="97"/>
-      <c r="P50" s="129"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="170"/>
+      <c r="P50" s="136"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="59"/>
       <c r="S50" s="97"/>
-      <c r="T50" s="129"/>
-      <c r="U50" s="70"/>
+      <c r="T50" s="136"/>
+      <c r="U50" s="36"/>
       <c r="V50" s="97"/>
-      <c r="W50" s="132" t="s">
-        <v>83</v>
-      </c>
-      <c r="X50" s="68" t="s">
-        <v>83</v>
-      </c>
+      <c r="W50" s="129"/>
+      <c r="X50" s="88"/>
     </row>
     <row r="51" spans="1:24">
-      <c r="A51" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="170"/>
-      <c r="C51" s="112"/>
-      <c r="D51" s="151"/>
+      <c r="B51" s="93"/>
+      <c r="C51" s="109"/>
+      <c r="D51" s="148"/>
       <c r="E51" s="97"/>
-      <c r="F51" s="135"/>
-      <c r="G51" s="36"/>
+      <c r="F51" s="133"/>
+      <c r="G51" s="27"/>
       <c r="H51" s="97"/>
-      <c r="I51" s="170"/>
-      <c r="J51" s="36"/>
+      <c r="I51" s="93"/>
+      <c r="J51" s="27"/>
       <c r="K51" s="97"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="170"/>
-      <c r="N51" s="78"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="90"/>
+      <c r="N51" s="31"/>
       <c r="O51" s="97"/>
-      <c r="P51" s="135"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="170"/>
+      <c r="P51" s="130"/>
+      <c r="R51" s="90"/>
       <c r="S51" s="97"/>
-      <c r="T51" s="135"/>
-      <c r="U51" s="70"/>
+      <c r="T51" s="130"/>
+      <c r="U51" s="31"/>
       <c r="V51" s="97"/>
-      <c r="W51" s="135"/>
-      <c r="X51" s="36"/>
-    </row>
-    <row r="52" spans="1:24">
-      <c r="A52" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="170"/>
-      <c r="C52" s="116"/>
-      <c r="D52" s="153"/>
-      <c r="E52" s="97"/>
-      <c r="F52" s="129"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="97"/>
-      <c r="I52" s="170"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="97"/>
-      <c r="L52" s="41"/>
-      <c r="M52" s="170"/>
-      <c r="N52" s="78"/>
-      <c r="O52" s="97"/>
-      <c r="P52" s="129"/>
-      <c r="Q52" s="13"/>
-      <c r="R52" s="170"/>
-      <c r="S52" s="97"/>
-      <c r="T52" s="129"/>
-      <c r="U52" s="70"/>
-      <c r="V52" s="97"/>
-      <c r="W52" s="135"/>
-      <c r="X52" s="36"/>
-    </row>
-    <row r="53" spans="1:24">
-      <c r="A53" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="170"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="153"/>
-      <c r="E53" s="97"/>
-      <c r="F53" s="135"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="97"/>
-      <c r="I53" s="170"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="97"/>
-      <c r="L53" s="41"/>
-      <c r="M53" s="170"/>
-      <c r="N53" s="78"/>
-      <c r="O53" s="97"/>
-      <c r="P53" s="135"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="170"/>
-      <c r="S53" s="97"/>
-      <c r="T53" s="135"/>
+      <c r="W51" s="130"/>
+      <c r="X51" s="31"/>
+    </row>
+    <row r="52" spans="1:24" s="52" customFormat="1">
+      <c r="A52" s="162" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="168"/>
+      <c r="C52" s="119"/>
+      <c r="D52" s="157"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="134"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="48"/>
+      <c r="N52" s="53"/>
+      <c r="O52" s="48"/>
+      <c r="P52" s="134"/>
+      <c r="R52" s="48"/>
+      <c r="S52" s="48"/>
+      <c r="T52" s="134"/>
+      <c r="U52" s="53"/>
+      <c r="V52" s="48"/>
+      <c r="W52" s="134"/>
+      <c r="X52" s="53"/>
+    </row>
+    <row r="53" spans="1:24" s="1" customFormat="1">
+      <c r="A53" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="169"/>
+      <c r="C53" s="120"/>
+      <c r="D53" s="148" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="99"/>
+      <c r="F53" s="137"/>
+      <c r="G53" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H53" s="99"/>
+      <c r="I53" s="169"/>
+      <c r="J53" s="70"/>
+      <c r="K53" s="99"/>
+      <c r="L53" s="40"/>
+      <c r="M53" s="169"/>
+      <c r="N53" s="70"/>
+      <c r="O53" s="99"/>
+      <c r="P53" s="137"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="169"/>
+      <c r="S53" s="99"/>
+      <c r="T53" s="137"/>
       <c r="U53" s="70"/>
-      <c r="V53" s="97"/>
-      <c r="W53" s="129"/>
-      <c r="X53" s="34"/>
+      <c r="V53" s="99"/>
+      <c r="W53" s="137"/>
+      <c r="X53" s="27" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="54" spans="1:24">
+      <c r="A54" s="9"/>
       <c r="B54" s="93"/>
-      <c r="C54" s="117"/>
-      <c r="D54" s="154"/>
+      <c r="C54" s="109"/>
+      <c r="D54" s="148"/>
       <c r="E54" s="97"/>
-      <c r="F54" s="131"/>
-      <c r="G54" s="38"/>
+      <c r="F54" s="130"/>
+      <c r="G54" s="31"/>
       <c r="H54" s="97"/>
       <c r="I54" s="93"/>
-      <c r="J54" s="38"/>
+      <c r="J54" s="31"/>
       <c r="K54" s="97"/>
       <c r="L54" s="30"/>
       <c r="M54" s="90"/>
@@ -3625,103 +3640,98 @@
       <c r="X54" s="31"/>
     </row>
     <row r="55" spans="1:24">
-      <c r="A55" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="93"/>
-      <c r="C55" s="117"/>
-      <c r="D55" s="154"/>
+      <c r="A55" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="169"/>
+      <c r="C55" s="112"/>
+      <c r="D55" s="151"/>
       <c r="E55" s="97"/>
-      <c r="F55" s="131"/>
-      <c r="G55" s="38"/>
+      <c r="F55" s="129"/>
+      <c r="G55" s="34"/>
       <c r="H55" s="97"/>
-      <c r="I55" s="93"/>
-      <c r="J55" s="38"/>
+      <c r="I55" s="170"/>
+      <c r="J55" s="36"/>
       <c r="K55" s="97"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="90"/>
-      <c r="N55" s="31"/>
+      <c r="L55" s="41"/>
+      <c r="M55" s="170"/>
+      <c r="N55" s="78"/>
       <c r="O55" s="97"/>
-      <c r="P55" s="130"/>
-      <c r="R55" s="90"/>
+      <c r="P55" s="129"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="170"/>
       <c r="S55" s="97"/>
-      <c r="T55" s="130"/>
-      <c r="U55" s="31"/>
+      <c r="T55" s="129"/>
+      <c r="U55" s="70"/>
       <c r="V55" s="97"/>
-      <c r="W55" s="130"/>
-      <c r="X55" s="31"/>
+      <c r="W55" s="129"/>
+      <c r="X55" s="34"/>
     </row>
     <row r="56" spans="1:24">
       <c r="A56" s="8" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B56" s="170"/>
-      <c r="C56" s="115" t="s">
-        <v>50</v>
-      </c>
-      <c r="D56" s="153"/>
+      <c r="C56" s="112"/>
+      <c r="D56" s="151"/>
       <c r="E56" s="97"/>
-      <c r="F56" s="135"/>
-      <c r="G56" s="36"/>
+      <c r="F56" s="129"/>
+      <c r="G56" s="34"/>
       <c r="H56" s="97"/>
       <c r="I56" s="170"/>
-      <c r="J56" s="36"/>
+      <c r="J56" s="34"/>
       <c r="K56" s="97"/>
       <c r="L56" s="41"/>
       <c r="M56" s="170"/>
       <c r="N56" s="78"/>
       <c r="O56" s="97"/>
-      <c r="P56" s="135"/>
-      <c r="Q56" s="15"/>
+      <c r="P56" s="129"/>
+      <c r="Q56" s="13"/>
       <c r="R56" s="170"/>
       <c r="S56" s="97"/>
-      <c r="T56" s="135"/>
+      <c r="T56" s="129"/>
       <c r="U56" s="70"/>
       <c r="V56" s="97"/>
-      <c r="W56" s="135"/>
-      <c r="X56" s="36"/>
+      <c r="W56" s="129"/>
+      <c r="X56" s="34"/>
     </row>
     <row r="57" spans="1:24">
-      <c r="A57" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="170"/>
-      <c r="C57" s="112"/>
-      <c r="D57" s="151"/>
+      <c r="B57" s="93"/>
+      <c r="C57" s="117"/>
+      <c r="D57" s="154"/>
       <c r="E57" s="97"/>
-      <c r="F57" s="129"/>
-      <c r="G57" s="34"/>
+      <c r="F57" s="131"/>
+      <c r="G57" s="38"/>
       <c r="H57" s="97"/>
-      <c r="I57" s="170"/>
-      <c r="J57" s="36"/>
+      <c r="I57" s="93"/>
+      <c r="J57" s="38"/>
       <c r="K57" s="97"/>
-      <c r="L57" s="41"/>
-      <c r="M57" s="170"/>
-      <c r="N57" s="78"/>
+      <c r="L57" s="30"/>
+      <c r="M57" s="90"/>
+      <c r="N57" s="31"/>
       <c r="O57" s="97"/>
-      <c r="P57" s="129"/>
-      <c r="Q57" s="13"/>
-      <c r="R57" s="170"/>
+      <c r="P57" s="130"/>
+      <c r="R57" s="90"/>
       <c r="S57" s="97"/>
-      <c r="T57" s="129"/>
-      <c r="U57" s="70"/>
+      <c r="T57" s="130"/>
+      <c r="U57" s="31"/>
       <c r="V57" s="97"/>
-      <c r="W57" s="129"/>
-      <c r="X57" s="34"/>
+      <c r="W57" s="130"/>
+      <c r="X57" s="31"/>
     </row>
     <row r="58" spans="1:24">
       <c r="A58" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B58" s="170"/>
-      <c r="C58" s="112"/>
-      <c r="D58" s="151"/>
+      <c r="C58" s="116"/>
+      <c r="D58" s="153"/>
       <c r="E58" s="97"/>
       <c r="F58" s="129"/>
       <c r="G58" s="34"/>
       <c r="H58" s="97"/>
       <c r="I58" s="170"/>
-      <c r="J58" s="34"/>
+      <c r="J58" s="36"/>
       <c r="K58" s="97"/>
       <c r="L58" s="41"/>
       <c r="M58" s="170"/>
@@ -3734,19 +3744,23 @@
       <c r="T58" s="129"/>
       <c r="U58" s="70"/>
       <c r="V58" s="97"/>
-      <c r="W58" s="129"/>
-      <c r="X58" s="34"/>
+      <c r="W58" s="132" t="s">
+        <v>83</v>
+      </c>
+      <c r="X58" s="68" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="59" spans="1:24">
       <c r="A59" s="8" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B59" s="170"/>
       <c r="C59" s="112"/>
-      <c r="D59" s="153"/>
+      <c r="D59" s="151"/>
       <c r="E59" s="97"/>
-      <c r="F59" s="129"/>
-      <c r="G59" s="34"/>
+      <c r="F59" s="135"/>
+      <c r="G59" s="36"/>
       <c r="H59" s="97"/>
       <c r="I59" s="170"/>
       <c r="J59" s="36"/>
@@ -3755,895 +3769,1116 @@
       <c r="M59" s="170"/>
       <c r="N59" s="78"/>
       <c r="O59" s="97"/>
-      <c r="P59" s="129"/>
-      <c r="Q59" s="13"/>
+      <c r="P59" s="135"/>
+      <c r="Q59" s="15"/>
       <c r="R59" s="170"/>
       <c r="S59" s="97"/>
-      <c r="T59" s="129"/>
+      <c r="T59" s="135"/>
       <c r="U59" s="70"/>
       <c r="V59" s="97"/>
-      <c r="W59" s="129"/>
-      <c r="X59" s="34"/>
+      <c r="W59" s="135"/>
+      <c r="X59" s="36"/>
     </row>
     <row r="60" spans="1:24">
-      <c r="B60" s="93"/>
-      <c r="C60" s="117"/>
-      <c r="D60" s="154"/>
+      <c r="A60" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="170"/>
+      <c r="C60" s="116"/>
+      <c r="D60" s="153"/>
       <c r="E60" s="97"/>
-      <c r="F60" s="131"/>
-      <c r="G60" s="38"/>
+      <c r="F60" s="129"/>
+      <c r="G60" s="34"/>
       <c r="H60" s="97"/>
-      <c r="I60" s="89"/>
-      <c r="J60" s="38"/>
+      <c r="I60" s="170"/>
+      <c r="J60" s="36"/>
       <c r="K60" s="97"/>
-      <c r="L60" s="30"/>
-      <c r="M60" s="90"/>
-      <c r="N60" s="31"/>
+      <c r="L60" s="41"/>
+      <c r="M60" s="170"/>
+      <c r="N60" s="78"/>
       <c r="O60" s="97"/>
-      <c r="P60" s="130"/>
-      <c r="R60" s="90"/>
+      <c r="P60" s="129"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="170"/>
       <c r="S60" s="97"/>
-      <c r="T60" s="130"/>
-      <c r="U60" s="31"/>
+      <c r="T60" s="129"/>
+      <c r="U60" s="70"/>
       <c r="V60" s="97"/>
-      <c r="W60" s="130"/>
-      <c r="X60" s="31"/>
-    </row>
-    <row r="61" spans="1:24" s="56" customFormat="1">
-      <c r="A61" s="162" t="s">
+      <c r="W60" s="135"/>
+      <c r="X60" s="36"/>
+    </row>
+    <row r="61" spans="1:24">
+      <c r="A61" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="170"/>
+      <c r="C61" s="116"/>
+      <c r="D61" s="153"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="135"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="97"/>
+      <c r="I61" s="170"/>
+      <c r="J61" s="36"/>
+      <c r="K61" s="97"/>
+      <c r="L61" s="41"/>
+      <c r="M61" s="170"/>
+      <c r="N61" s="78"/>
+      <c r="O61" s="97"/>
+      <c r="P61" s="135"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="170"/>
+      <c r="S61" s="97"/>
+      <c r="T61" s="135"/>
+      <c r="U61" s="70"/>
+      <c r="V61" s="97"/>
+      <c r="W61" s="129"/>
+      <c r="X61" s="34"/>
+    </row>
+    <row r="62" spans="1:24">
+      <c r="B62" s="93"/>
+      <c r="C62" s="117"/>
+      <c r="D62" s="154"/>
+      <c r="E62" s="97"/>
+      <c r="F62" s="131"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="97"/>
+      <c r="I62" s="93"/>
+      <c r="J62" s="38"/>
+      <c r="K62" s="97"/>
+      <c r="L62" s="30"/>
+      <c r="M62" s="90"/>
+      <c r="N62" s="31"/>
+      <c r="O62" s="97"/>
+      <c r="P62" s="130"/>
+      <c r="R62" s="90"/>
+      <c r="S62" s="97"/>
+      <c r="T62" s="130"/>
+      <c r="U62" s="31"/>
+      <c r="V62" s="97"/>
+      <c r="W62" s="130"/>
+      <c r="X62" s="31"/>
+    </row>
+    <row r="63" spans="1:24">
+      <c r="A63" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63" s="93"/>
+      <c r="C63" s="117"/>
+      <c r="D63" s="154"/>
+      <c r="E63" s="97"/>
+      <c r="F63" s="131"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="97"/>
+      <c r="I63" s="93"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="97"/>
+      <c r="L63" s="30"/>
+      <c r="M63" s="90"/>
+      <c r="N63" s="31"/>
+      <c r="O63" s="97"/>
+      <c r="P63" s="130"/>
+      <c r="R63" s="90"/>
+      <c r="S63" s="97"/>
+      <c r="T63" s="130"/>
+      <c r="U63" s="31"/>
+      <c r="V63" s="97"/>
+      <c r="W63" s="130"/>
+      <c r="X63" s="31"/>
+    </row>
+    <row r="64" spans="1:24">
+      <c r="A64" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" s="170"/>
+      <c r="C64" s="115" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="153"/>
+      <c r="E64" s="97"/>
+      <c r="F64" s="135"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="97"/>
+      <c r="I64" s="170"/>
+      <c r="J64" s="36"/>
+      <c r="K64" s="97"/>
+      <c r="L64" s="41"/>
+      <c r="M64" s="170"/>
+      <c r="N64" s="78"/>
+      <c r="O64" s="97"/>
+      <c r="P64" s="135"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="170"/>
+      <c r="S64" s="97"/>
+      <c r="T64" s="135"/>
+      <c r="U64" s="70"/>
+      <c r="V64" s="97"/>
+      <c r="W64" s="135"/>
+      <c r="X64" s="36"/>
+    </row>
+    <row r="65" spans="1:24">
+      <c r="A65" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="170"/>
+      <c r="C65" s="112"/>
+      <c r="D65" s="151"/>
+      <c r="E65" s="97"/>
+      <c r="F65" s="129"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="97"/>
+      <c r="I65" s="170"/>
+      <c r="J65" s="36"/>
+      <c r="K65" s="97"/>
+      <c r="L65" s="41"/>
+      <c r="M65" s="170"/>
+      <c r="N65" s="78"/>
+      <c r="O65" s="97"/>
+      <c r="P65" s="129"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="170"/>
+      <c r="S65" s="97"/>
+      <c r="T65" s="129"/>
+      <c r="U65" s="70"/>
+      <c r="V65" s="97"/>
+      <c r="W65" s="129"/>
+      <c r="X65" s="34"/>
+    </row>
+    <row r="66" spans="1:24">
+      <c r="A66" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="170"/>
+      <c r="C66" s="112"/>
+      <c r="D66" s="151"/>
+      <c r="E66" s="97"/>
+      <c r="F66" s="129"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="97"/>
+      <c r="I66" s="170"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="97"/>
+      <c r="L66" s="41"/>
+      <c r="M66" s="170"/>
+      <c r="N66" s="78"/>
+      <c r="O66" s="97"/>
+      <c r="P66" s="129"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="170"/>
+      <c r="S66" s="97"/>
+      <c r="T66" s="129"/>
+      <c r="U66" s="70"/>
+      <c r="V66" s="97"/>
+      <c r="W66" s="129"/>
+      <c r="X66" s="34"/>
+    </row>
+    <row r="67" spans="1:24">
+      <c r="A67" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="170"/>
+      <c r="C67" s="112"/>
+      <c r="D67" s="153"/>
+      <c r="E67" s="97"/>
+      <c r="F67" s="129"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="97"/>
+      <c r="I67" s="170"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="97"/>
+      <c r="L67" s="41"/>
+      <c r="M67" s="170"/>
+      <c r="N67" s="78"/>
+      <c r="O67" s="97"/>
+      <c r="P67" s="129"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="170"/>
+      <c r="S67" s="97"/>
+      <c r="T67" s="129"/>
+      <c r="U67" s="70"/>
+      <c r="V67" s="97"/>
+      <c r="W67" s="129"/>
+      <c r="X67" s="34"/>
+    </row>
+    <row r="68" spans="1:24">
+      <c r="B68" s="93"/>
+      <c r="C68" s="117"/>
+      <c r="D68" s="154"/>
+      <c r="E68" s="97"/>
+      <c r="F68" s="131"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="97"/>
+      <c r="I68" s="89"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="97"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="90"/>
+      <c r="N68" s="31"/>
+      <c r="O68" s="97"/>
+      <c r="P68" s="130"/>
+      <c r="R68" s="90"/>
+      <c r="S68" s="97"/>
+      <c r="T68" s="130"/>
+      <c r="U68" s="31"/>
+      <c r="V68" s="97"/>
+      <c r="W68" s="130"/>
+      <c r="X68" s="31"/>
+    </row>
+    <row r="69" spans="1:24" s="56" customFormat="1">
+      <c r="A69" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="95" t="s">
+      <c r="B69" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="121" t="s">
+      <c r="C69" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="D61" s="158" t="s">
+      <c r="D69" s="158" t="s">
         <v>13</v>
       </c>
-      <c r="E61" s="47"/>
-      <c r="F61" s="138" t="s">
+      <c r="E69" s="47"/>
+      <c r="F69" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="G61" s="55" t="s">
+      <c r="G69" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="H61" s="47"/>
-      <c r="I61" s="95" t="s">
+      <c r="H69" s="47"/>
+      <c r="I69" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="J61" s="55" t="s">
+      <c r="J69" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="K61" s="47"/>
-      <c r="L61" s="65" t="s">
+      <c r="K69" s="47"/>
+      <c r="L69" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="M61" s="95" t="s">
+      <c r="M69" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="N61" s="55" t="s">
+      <c r="N69" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="O61" s="47"/>
-      <c r="P61" s="138" t="s">
+      <c r="O69" s="47"/>
+      <c r="P69" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="Q61" s="54" t="s">
+      <c r="Q69" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="R61" s="95" t="s">
+      <c r="R69" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="S61" s="47"/>
-      <c r="T61" s="138" t="s">
+      <c r="S69" s="47"/>
+      <c r="T69" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="U61" s="55" t="s">
+      <c r="U69" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="V61" s="47"/>
-      <c r="W61" s="138" t="s">
+      <c r="V69" s="47"/>
+      <c r="W69" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="X61" s="55" t="s">
+      <c r="X69" s="55" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
-      <c r="A62" s="8">
+    <row r="70" spans="1:24">
+      <c r="A70" s="8">
         <v>10</v>
       </c>
-      <c r="B62" s="171">
+      <c r="B70" s="171">
         <v>10</v>
       </c>
-      <c r="C62" s="122">
+      <c r="C70" s="122">
         <v>10</v>
       </c>
-      <c r="D62" s="159">
+      <c r="D70" s="159">
         <v>1000</v>
       </c>
-      <c r="E62" s="100"/>
-      <c r="F62" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G62" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H62" s="100"/>
-      <c r="I62" s="171">
+      <c r="E70" s="100"/>
+      <c r="F70" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70" s="100"/>
+      <c r="I70" s="171">
         <v>180</v>
       </c>
-      <c r="J62" s="43">
+      <c r="J70" s="43">
         <v>1000</v>
       </c>
-      <c r="K62" s="100"/>
-      <c r="L62" s="42">
+      <c r="K70" s="100"/>
+      <c r="L70" s="42">
         <v>150</v>
       </c>
-      <c r="M62" s="171">
-        <f t="shared" ref="M62:M72" si="1">A62*35</f>
+      <c r="M70" s="171">
+        <f t="shared" ref="M70:M80" si="1">A70*35</f>
         <v>350</v>
       </c>
-      <c r="N62" s="43">
-        <f t="shared" ref="N62:N72" si="2">A62*45</f>
+      <c r="N70" s="43">
+        <f t="shared" ref="N70:N80" si="2">A70*45</f>
         <v>450</v>
       </c>
-      <c r="O62" s="100"/>
-      <c r="P62" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q62" s="19">
+      <c r="O70" s="100"/>
+      <c r="P70" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q70" s="19">
         <v>2149</v>
       </c>
-      <c r="R62" s="180">
+      <c r="R70" s="180">
         <v>200</v>
       </c>
-      <c r="S62" s="100"/>
-      <c r="T62" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U62" s="27" t="s">
+      <c r="S70" s="100"/>
+      <c r="T70" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U70" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V62" s="100"/>
-      <c r="W62" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X62" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24">
-      <c r="A63" s="8">
+      <c r="V70" s="100"/>
+      <c r="W70" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X70" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24">
+      <c r="A71" s="8">
         <v>15</v>
       </c>
-      <c r="B63" s="171">
+      <c r="B71" s="171">
         <v>50</v>
       </c>
-      <c r="C63" s="122" t="s">
+      <c r="C71" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D63" s="159">
+      <c r="D71" s="159">
         <v>1500</v>
       </c>
-      <c r="E63" s="100"/>
-      <c r="F63" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G63" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H63" s="100"/>
-      <c r="I63" s="171" t="s">
+      <c r="E71" s="100"/>
+      <c r="F71" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H71" s="100"/>
+      <c r="I71" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="J63" s="43" t="s">
+      <c r="J71" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K63" s="100"/>
-      <c r="L63" s="42">
+      <c r="K71" s="100"/>
+      <c r="L71" s="42">
         <v>225</v>
       </c>
-      <c r="M63" s="171">
+      <c r="M71" s="171">
         <f t="shared" si="1"/>
         <v>525</v>
       </c>
-      <c r="N63" s="43">
+      <c r="N71" s="43">
         <f t="shared" si="2"/>
         <v>675</v>
       </c>
-      <c r="O63" s="100"/>
-      <c r="P63" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q63" s="19" t="s">
+      <c r="O71" s="100"/>
+      <c r="P71" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q71" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="R63" s="180">
+      <c r="R71" s="180">
         <v>300</v>
       </c>
-      <c r="S63" s="100"/>
-      <c r="T63" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U63" s="27" t="s">
+      <c r="S71" s="100"/>
+      <c r="T71" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U71" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V63" s="100"/>
-      <c r="W63" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X63" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24">
-      <c r="A64" s="8">
+      <c r="V71" s="100"/>
+      <c r="W71" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X71" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24">
+      <c r="A72" s="8">
         <v>20</v>
       </c>
-      <c r="B64" s="171" t="s">
+      <c r="B72" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="C64" s="122" t="s">
+      <c r="C72" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="159" t="s">
+      <c r="D72" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="100"/>
-      <c r="F64" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H64" s="100"/>
-      <c r="I64" s="171">
+      <c r="E72" s="100"/>
+      <c r="F72" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H72" s="100"/>
+      <c r="I72" s="171">
         <v>260</v>
       </c>
-      <c r="J64" s="43">
+      <c r="J72" s="43">
         <v>1800</v>
       </c>
-      <c r="K64" s="100"/>
-      <c r="L64" s="42">
+      <c r="K72" s="100"/>
+      <c r="L72" s="42">
         <v>300</v>
       </c>
-      <c r="M64" s="171">
+      <c r="M72" s="171">
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
-      <c r="N64" s="43">
+      <c r="N72" s="43">
         <f t="shared" si="2"/>
         <v>900</v>
       </c>
-      <c r="O64" s="100"/>
-      <c r="P64" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q64" s="19" t="s">
+      <c r="O72" s="100"/>
+      <c r="P72" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q72" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="R64" s="180">
+      <c r="R72" s="180">
         <v>400</v>
       </c>
-      <c r="S64" s="100"/>
-      <c r="T64" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U64" s="27" t="s">
+      <c r="S72" s="100"/>
+      <c r="T72" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U72" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V64" s="100"/>
-      <c r="W64" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X64" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24">
-      <c r="A65" s="8">
+      <c r="V72" s="100"/>
+      <c r="W72" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X72" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24">
+      <c r="A73" s="8">
         <v>25</v>
       </c>
-      <c r="B65" s="171">
+      <c r="B73" s="171">
         <v>100</v>
       </c>
-      <c r="C65" s="122">
+      <c r="C73" s="122">
         <v>1200</v>
       </c>
-      <c r="D65" s="159">
+      <c r="D73" s="159">
         <v>2000</v>
       </c>
-      <c r="E65" s="100"/>
-      <c r="F65" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G65" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H65" s="100"/>
-      <c r="I65" s="171" t="s">
+      <c r="E73" s="100"/>
+      <c r="F73" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H73" s="100"/>
+      <c r="I73" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="J65" s="43" t="s">
+      <c r="J73" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K65" s="100"/>
-      <c r="L65" s="42">
+      <c r="K73" s="100"/>
+      <c r="L73" s="42">
         <v>375</v>
       </c>
-      <c r="M65" s="171">
+      <c r="M73" s="171">
         <f t="shared" si="1"/>
         <v>875</v>
       </c>
-      <c r="N65" s="43">
+      <c r="N73" s="43">
         <f t="shared" si="2"/>
         <v>1125</v>
       </c>
-      <c r="O65" s="100"/>
-      <c r="P65" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q65" s="19">
+      <c r="O73" s="100"/>
+      <c r="P73" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q73" s="19">
         <v>4799</v>
       </c>
-      <c r="R65" s="180">
+      <c r="R73" s="180">
         <v>449</v>
       </c>
-      <c r="S65" s="100"/>
-      <c r="T65" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U65" s="27" t="s">
+      <c r="S73" s="100"/>
+      <c r="T73" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U73" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V65" s="100"/>
-      <c r="W65" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X65" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:24">
-      <c r="A66" s="8">
+      <c r="V73" s="100"/>
+      <c r="W73" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X73" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24">
+      <c r="A74" s="8">
         <v>30</v>
       </c>
-      <c r="B66" s="171" t="s">
+      <c r="B74" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="122" t="s">
+      <c r="C74" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="159" t="s">
+      <c r="D74" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="E66" s="100"/>
-      <c r="F66" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G66" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H66" s="100"/>
-      <c r="I66" s="171">
+      <c r="E74" s="100"/>
+      <c r="F74" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G74" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H74" s="100"/>
+      <c r="I74" s="171">
         <v>300</v>
       </c>
-      <c r="J66" s="43" t="s">
+      <c r="J74" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K66" s="100"/>
-      <c r="L66" s="42">
+      <c r="K74" s="100"/>
+      <c r="L74" s="42">
         <v>450</v>
       </c>
-      <c r="M66" s="171">
+      <c r="M74" s="171">
         <f t="shared" si="1"/>
         <v>1050</v>
       </c>
-      <c r="N66" s="43">
+      <c r="N74" s="43">
         <f t="shared" si="2"/>
         <v>1350</v>
       </c>
-      <c r="O66" s="100"/>
-      <c r="P66" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q66" s="19" t="s">
+      <c r="O74" s="100"/>
+      <c r="P74" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q74" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="R66" s="180">
+      <c r="R74" s="180">
         <v>449</v>
       </c>
-      <c r="S66" s="100"/>
-      <c r="T66" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U66" s="27" t="s">
+      <c r="S74" s="100"/>
+      <c r="T74" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U74" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V66" s="100"/>
-      <c r="W66" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X66" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24">
-      <c r="A67" s="8">
+      <c r="V74" s="100"/>
+      <c r="W74" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X74" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24">
+      <c r="A75" s="8">
         <v>50</v>
       </c>
-      <c r="B67" s="171">
+      <c r="B75" s="171">
         <v>200</v>
       </c>
-      <c r="C67" s="122">
+      <c r="C75" s="122">
         <v>2200</v>
       </c>
-      <c r="D67" s="159">
+      <c r="D75" s="159">
         <v>4000</v>
       </c>
-      <c r="E67" s="100"/>
-      <c r="F67" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G67" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H67" s="100"/>
-      <c r="I67" s="171">
+      <c r="E75" s="100"/>
+      <c r="F75" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G75" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H75" s="100"/>
+      <c r="I75" s="171">
         <v>360</v>
       </c>
-      <c r="J67" s="43">
+      <c r="J75" s="43">
         <v>3000</v>
       </c>
-      <c r="K67" s="100"/>
-      <c r="L67" s="42">
+      <c r="K75" s="100"/>
+      <c r="L75" s="42">
         <v>750</v>
       </c>
-      <c r="M67" s="171">
+      <c r="M75" s="171">
         <f t="shared" si="1"/>
         <v>1750</v>
       </c>
-      <c r="N67" s="43">
+      <c r="N75" s="43">
         <f t="shared" si="2"/>
         <v>2250</v>
       </c>
-      <c r="O67" s="100"/>
-      <c r="P67" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q67" s="19">
+      <c r="O75" s="100"/>
+      <c r="P75" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q75" s="19">
         <v>6999</v>
       </c>
-      <c r="R67" s="180">
+      <c r="R75" s="180">
         <v>629</v>
       </c>
-      <c r="S67" s="100"/>
-      <c r="T67" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U67" s="27" t="s">
+      <c r="S75" s="100"/>
+      <c r="T75" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U75" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V67" s="100"/>
-      <c r="W67" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X67" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24">
-      <c r="A68" s="8">
+      <c r="V75" s="100"/>
+      <c r="W75" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X75" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24">
+      <c r="A76" s="8">
         <v>100</v>
       </c>
-      <c r="B68" s="171">
+      <c r="B76" s="171">
         <v>300</v>
       </c>
-      <c r="C68" s="122">
+      <c r="C76" s="122">
         <v>4000</v>
       </c>
-      <c r="D68" s="159">
+      <c r="D76" s="159">
         <v>8000</v>
       </c>
-      <c r="E68" s="100"/>
-      <c r="F68" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G68" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H68" s="100"/>
-      <c r="I68" s="171">
+      <c r="E76" s="100"/>
+      <c r="F76" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G76" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H76" s="100"/>
+      <c r="I76" s="171">
         <v>500</v>
       </c>
-      <c r="J68" s="43">
+      <c r="J76" s="43">
         <v>5000</v>
       </c>
-      <c r="K68" s="100"/>
-      <c r="L68" s="42">
+      <c r="K76" s="100"/>
+      <c r="L76" s="42">
         <v>1500</v>
       </c>
-      <c r="M68" s="171">
+      <c r="M76" s="171">
         <f t="shared" si="1"/>
         <v>3500</v>
       </c>
-      <c r="N68" s="43">
+      <c r="N76" s="43">
         <f t="shared" si="2"/>
         <v>4500</v>
       </c>
-      <c r="O68" s="100"/>
-      <c r="P68" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q68" s="19">
+      <c r="O76" s="100"/>
+      <c r="P76" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q76" s="19">
         <v>9999</v>
       </c>
-      <c r="R68" s="180">
+      <c r="R76" s="180">
         <v>1149</v>
       </c>
-      <c r="S68" s="100"/>
-      <c r="T68" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U68" s="27" t="s">
+      <c r="S76" s="100"/>
+      <c r="T76" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U76" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V68" s="100"/>
-      <c r="W68" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X68" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24">
-      <c r="A69" s="8">
+      <c r="V76" s="100"/>
+      <c r="W76" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X76" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24">
+      <c r="A77" s="8">
         <v>250</v>
       </c>
-      <c r="B69" s="171" t="s">
+      <c r="B77" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="122">
+      <c r="C77" s="122">
         <v>8000</v>
       </c>
-      <c r="D69" s="159" t="s">
+      <c r="D77" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="100"/>
-      <c r="F69" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G69" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H69" s="100"/>
-      <c r="I69" s="171">
+      <c r="E77" s="100"/>
+      <c r="F77" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G77" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H77" s="100"/>
+      <c r="I77" s="171">
         <v>800</v>
       </c>
-      <c r="J69" s="43" t="s">
+      <c r="J77" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K69" s="100"/>
-      <c r="L69" s="42">
+      <c r="K77" s="100"/>
+      <c r="L77" s="42">
         <v>3750</v>
       </c>
-      <c r="M69" s="171">
+      <c r="M77" s="171">
         <f t="shared" si="1"/>
         <v>8750</v>
       </c>
-      <c r="N69" s="43">
+      <c r="N77" s="43">
         <f t="shared" si="2"/>
         <v>11250</v>
       </c>
-      <c r="O69" s="100"/>
-      <c r="P69" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q69" s="19" t="s">
+      <c r="O77" s="100"/>
+      <c r="P77" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q77" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="R69" s="180">
+      <c r="R77" s="180">
         <v>1999</v>
       </c>
-      <c r="S69" s="100"/>
-      <c r="T69" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U69" s="27" t="s">
+      <c r="S77" s="100"/>
+      <c r="T77" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U77" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V69" s="100"/>
-      <c r="W69" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X69" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24">
-      <c r="A70" s="8">
+      <c r="V77" s="100"/>
+      <c r="W77" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X77" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24">
+      <c r="A78" s="8">
         <v>500</v>
       </c>
-      <c r="B70" s="171">
+      <c r="B78" s="171">
         <v>500</v>
       </c>
-      <c r="C70" s="122">
+      <c r="C78" s="122">
         <v>12000</v>
       </c>
-      <c r="D70" s="159" t="s">
+      <c r="D78" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="100"/>
-      <c r="F70" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G70" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H70" s="100"/>
-      <c r="I70" s="171">
+      <c r="E78" s="100"/>
+      <c r="F78" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G78" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" s="100"/>
+      <c r="I78" s="171">
         <v>900</v>
       </c>
-      <c r="J70" s="43" t="s">
+      <c r="J78" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K70" s="100"/>
-      <c r="L70" s="42">
+      <c r="K78" s="100"/>
+      <c r="L78" s="42">
         <v>7500</v>
       </c>
-      <c r="M70" s="171">
+      <c r="M78" s="171">
         <f t="shared" si="1"/>
         <v>17500</v>
       </c>
-      <c r="N70" s="43">
+      <c r="N78" s="43">
         <f t="shared" si="2"/>
         <v>22500</v>
       </c>
-      <c r="O70" s="100"/>
-      <c r="P70" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q70" s="19" t="s">
+      <c r="O78" s="100"/>
+      <c r="P78" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q78" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="R70" s="180" t="s">
+      <c r="R78" s="180" t="s">
         <v>19</v>
       </c>
-      <c r="S70" s="100"/>
-      <c r="T70" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U70" s="27" t="s">
+      <c r="S78" s="100"/>
+      <c r="T78" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U78" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V70" s="100"/>
-      <c r="W70" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X70" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24">
-      <c r="A71" s="8">
+      <c r="V78" s="100"/>
+      <c r="W78" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X78" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24">
+      <c r="A79" s="8">
         <v>2000</v>
       </c>
-      <c r="B71" s="171">
+      <c r="B79" s="171">
         <v>1000</v>
       </c>
-      <c r="C71" s="122">
+      <c r="C79" s="122">
         <v>16000</v>
       </c>
-      <c r="D71" s="159" t="s">
+      <c r="D79" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="100"/>
-      <c r="F71" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H71" s="100"/>
-      <c r="I71" s="171" t="s">
+      <c r="E79" s="100"/>
+      <c r="F79" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G79" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79" s="100"/>
+      <c r="I79" s="171" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="43" t="s">
+      <c r="J79" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K71" s="100"/>
-      <c r="L71" s="42">
+      <c r="K79" s="100"/>
+      <c r="L79" s="42">
         <v>30000</v>
       </c>
-      <c r="M71" s="171">
+      <c r="M79" s="171">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="N71" s="43">
+      <c r="N79" s="43">
         <f t="shared" si="2"/>
         <v>90000</v>
       </c>
-      <c r="O71" s="100"/>
-      <c r="P71" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q71" s="19" t="s">
+      <c r="O79" s="100"/>
+      <c r="P79" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q79" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="R71" s="180" t="s">
+      <c r="R79" s="180" t="s">
         <v>19</v>
       </c>
-      <c r="S71" s="100"/>
-      <c r="T71" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U71" s="27" t="s">
+      <c r="S79" s="100"/>
+      <c r="T79" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U79" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V71" s="100"/>
-      <c r="W71" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X71" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24">
-      <c r="A72" s="8">
+      <c r="V79" s="100"/>
+      <c r="W79" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X79" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24">
+      <c r="A80" s="8">
         <v>10000</v>
       </c>
-      <c r="B72" s="171" t="s">
+      <c r="B80" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="122">
+      <c r="C80" s="122">
         <v>20000</v>
       </c>
-      <c r="D72" s="159" t="s">
+      <c r="D80" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="E72" s="100"/>
-      <c r="F72" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="G72" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H72" s="100"/>
-      <c r="I72" s="171" t="s">
+      <c r="E80" s="100"/>
+      <c r="F80" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="G80" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H80" s="100"/>
+      <c r="I80" s="171" t="s">
         <v>19</v>
       </c>
-      <c r="J72" s="43" t="s">
+      <c r="J80" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K72" s="100"/>
-      <c r="L72" s="42">
+      <c r="K80" s="100"/>
+      <c r="L80" s="42">
         <v>150000</v>
       </c>
-      <c r="M72" s="171">
+      <c r="M80" s="171">
         <f t="shared" si="1"/>
         <v>350000</v>
       </c>
-      <c r="N72" s="43">
+      <c r="N80" s="43">
         <f t="shared" si="2"/>
         <v>450000</v>
       </c>
-      <c r="O72" s="100"/>
-      <c r="P72" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q72" s="19" t="s">
+      <c r="O80" s="100"/>
+      <c r="P80" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q80" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="R72" s="180" t="s">
+      <c r="R80" s="180" t="s">
         <v>19</v>
       </c>
-      <c r="S72" s="100"/>
-      <c r="T72" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="U72" s="27" t="s">
+      <c r="S80" s="100"/>
+      <c r="T80" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="U80" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="V72" s="100"/>
-      <c r="W72" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="X72" s="43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24">
-      <c r="A73" s="8" t="s">
+      <c r="V80" s="100"/>
+      <c r="W80" s="139" t="s">
+        <v>18</v>
+      </c>
+      <c r="X80" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24">
+      <c r="A81" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B73" s="172" t="s">
+      <c r="B81" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="123">
+      <c r="C81" s="123">
         <v>24000</v>
       </c>
-      <c r="D73" s="190" t="s">
+      <c r="D81" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="E73" s="101"/>
-      <c r="F73" s="140" t="s">
-        <v>18</v>
-      </c>
-      <c r="G73" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="H73" s="101"/>
-      <c r="I73" s="172" t="s">
+      <c r="E81" s="101"/>
+      <c r="F81" s="140" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81" s="101"/>
+      <c r="I81" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="J73" s="45">
+      <c r="J81" s="45">
         <v>7000</v>
       </c>
-      <c r="K73" s="101"/>
-      <c r="L73" s="44" t="s">
+      <c r="K81" s="101"/>
+      <c r="L81" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="M73" s="172" t="s">
+      <c r="M81" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="N73" s="45" t="s">
+      <c r="N81" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="O73" s="101"/>
-      <c r="P73" s="140" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q73" s="81" t="s">
+      <c r="O81" s="101"/>
+      <c r="P81" s="140" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q81" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="R73" s="181" t="s">
+      <c r="R81" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="S73" s="101"/>
-      <c r="T73" s="140" t="s">
-        <v>18</v>
-      </c>
-      <c r="U73" s="86" t="s">
+      <c r="S81" s="101"/>
+      <c r="T81" s="140" t="s">
+        <v>18</v>
+      </c>
+      <c r="U81" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="V73" s="101"/>
-      <c r="W73" s="140" t="s">
-        <v>18</v>
-      </c>
-      <c r="X73" s="45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24">
-      <c r="A74" s="47" t="s">
+      <c r="V81" s="101"/>
+      <c r="W81" s="140" t="s">
+        <v>18</v>
+      </c>
+      <c r="X81" s="45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24">
+      <c r="A82" s="47" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
-      <c r="A75" s="57" t="s">
+    <row r="83" spans="1:24">
+      <c r="A83" s="57" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:24">
-      <c r="A76" s="58" t="s">
+    <row r="84" spans="1:24">
+      <c r="A84" s="58" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
-      <c r="A77" s="59" t="s">
+    <row r="85" spans="1:24">
+      <c r="A85" s="59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:24">
-      <c r="A78" s="60" t="s">
+    <row r="86" spans="1:24">
+      <c r="A86" s="60" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:24">
-      <c r="A79" s="61" t="s">
+    <row r="87" spans="1:24">
+      <c r="A87" s="61" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4652,16 +4887,16 @@
     <sortCondition ref="A24:A28"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="W16:X16"/>
-    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>